<commit_message>
smx dp buttons added
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="113">
   <si>
     <t>Environment</t>
   </si>
@@ -343,6 +343,24 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>secondarylanguage</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>textbox</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Please fill the survey and help us improve!</t>
+  </si>
+  <si>
+    <t>Enter your Name</t>
   </si>
 </sst>
 </file>
@@ -897,11 +915,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:AV3"/>
+  <dimension ref="A1:AY3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AU4" sqref="AU4"/>
+      <selection pane="bottomLeft" activeCell="AY4" sqref="AY4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +937,7 @@
     <col min="11" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1064,8 +1082,17 @@
       <c r="AV1" s="7" t="s">
         <v>101</v>
       </c>
+      <c r="AW1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AY1" s="7" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1200,8 +1227,11 @@
       <c r="AT2" s="9"/>
       <c r="AU2" s="9"/>
       <c r="AV2" s="9"/>
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="9"/>
+      <c r="AY2" s="9"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -1272,6 +1302,15 @@
       <c r="AV3" s="9" t="s">
         <v>106</v>
       </c>
+      <c r="AW3" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX3" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="AY3" s="9" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
smx dp cases added
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="119">
   <si>
     <t>Environment</t>
   </si>
@@ -361,6 +361,24 @@
   </si>
   <si>
     <t>Enter your Name</t>
+  </si>
+  <si>
+    <t>radiobutton</t>
+  </si>
+  <si>
+    <t>AnswerOptions</t>
+  </si>
+  <si>
+    <t>Please select the options from the given list</t>
+  </si>
+  <si>
+    <t>Endorsement</t>
+  </si>
+  <si>
+    <t>checkbox</t>
+  </si>
+  <si>
+    <t>Please select your choices from the list</t>
   </si>
 </sst>
 </file>
@@ -915,11 +933,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:AY3"/>
+  <dimension ref="A1:BB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AY4" sqref="AY4"/>
+      <selection pane="bottomLeft" activeCell="BB3" sqref="BB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,7 +955,7 @@
     <col min="11" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1091,8 +1109,17 @@
       <c r="AY1" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="AZ1" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="BA1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="BB1" s="7" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1230,8 +1257,11 @@
       <c r="AW2" s="9"/>
       <c r="AX2" s="9"/>
       <c r="AY2" s="9"/>
+      <c r="AZ2" s="9"/>
+      <c r="BA2" s="9"/>
+      <c r="BB2" s="9"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -1311,6 +1341,15 @@
       <c r="AY3" s="9" t="s">
         <v>112</v>
       </c>
+      <c r="AZ3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="BA3" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="BB3" s="9" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
engage smx dp cases added
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="141">
   <si>
     <t>Environment</t>
   </si>
@@ -379,6 +379,72 @@
   </si>
   <si>
     <t>Please select your choices from the list</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start with a Blank Survey Button not present on page.</t>
+  </si>
+  <si>
+    <t>imagechoice</t>
+  </si>
+  <si>
+    <t>reportingvalue</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>likedislike</t>
+  </si>
+  <si>
+    <t>ratingscale</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>ranking</t>
+  </si>
+  <si>
+    <t>multitextbox</t>
+  </si>
+  <si>
+    <t>textbox1</t>
+  </si>
+  <si>
+    <t>textbox2</t>
+  </si>
+  <si>
+    <t>multidropdown</t>
+  </si>
+  <si>
+    <t>dropdown1</t>
+  </si>
+  <si>
+    <t>dropdown2</t>
+  </si>
+  <si>
+    <t>multiradio</t>
+  </si>
+  <si>
+    <t>QuestionOptions</t>
+  </si>
+  <si>
+    <t>multicheckbox</t>
+  </si>
+  <si>
+    <t>ratingradio</t>
+  </si>
+  <si>
+    <t>ratingdropdown</t>
+  </si>
+  <si>
+    <t>ratingscalegrid</t>
+  </si>
+  <si>
+    <t>matrixgrid</t>
   </si>
 </sst>
 </file>
@@ -411,11 +477,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -933,11 +1001,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:BB3"/>
+  <dimension ref="A1:BW3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BB3" sqref="BB3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +1023,7 @@
     <col min="11" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1118,8 +1186,71 @@
       <c r="BB1" s="7" t="s">
         <v>117</v>
       </c>
+      <c r="BC1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD1" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="BE1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="BF1" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="BG1" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="BH1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="BI1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="BK1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="BL1" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="BM1" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="BN1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="BO1" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="BP1" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="BQ1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="BR1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="BS1" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BT1" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="BU1" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="BV1" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="BW1" s="7" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1260,8 +1391,29 @@
       <c r="AZ2" s="9"/>
       <c r="BA2" s="9"/>
       <c r="BB2" s="9"/>
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="9"/>
+      <c r="BF2" s="9"/>
+      <c r="BG2" s="9"/>
+      <c r="BH2" s="9"/>
+      <c r="BI2" s="9"/>
+      <c r="BJ2" s="9"/>
+      <c r="BK2" s="9"/>
+      <c r="BL2" s="9"/>
+      <c r="BM2" s="9"/>
+      <c r="BN2" s="9"/>
+      <c r="BO2" s="9"/>
+      <c r="BP2" s="9"/>
+      <c r="BQ2" s="9"/>
+      <c r="BR2" s="9"/>
+      <c r="BS2" s="9"/>
+      <c r="BT2" s="9"/>
+      <c r="BU2" s="9"/>
+      <c r="BV2" s="9"/>
+      <c r="BW2" s="9"/>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -1287,7 +1439,9 @@
       <c r="I3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1350,6 +1504,27 @@
       <c r="BB3" s="9" t="s">
         <v>118</v>
       </c>
+      <c r="BC3" s="9"/>
+      <c r="BD3" s="9"/>
+      <c r="BE3" s="9"/>
+      <c r="BF3" s="9"/>
+      <c r="BG3" s="9"/>
+      <c r="BH3" s="9"/>
+      <c r="BI3" s="9"/>
+      <c r="BJ3" s="9"/>
+      <c r="BK3" s="9"/>
+      <c r="BL3" s="9"/>
+      <c r="BM3" s="9"/>
+      <c r="BN3" s="9"/>
+      <c r="BO3" s="9"/>
+      <c r="BP3" s="9"/>
+      <c r="BQ3" s="9"/>
+      <c r="BR3" s="9"/>
+      <c r="BS3" s="9"/>
+      <c r="BT3" s="9"/>
+      <c r="BU3" s="9"/>
+      <c r="BV3" s="9"/>
+      <c r="BW3" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
other smx cases added
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="147">
   <si>
     <t>Environment</t>
   </si>
@@ -445,6 +445,24 @@
   </si>
   <si>
     <t>matrixgrid</t>
+  </si>
+  <si>
+    <t>horizontalradiobutton</t>
+  </si>
+  <si>
+    <t>numericallocations</t>
+  </si>
+  <si>
+    <t>attachments</t>
+  </si>
+  <si>
+    <t>ratingradiobutton</t>
+  </si>
+  <si>
+    <t>ratingdropdownbutton</t>
+  </si>
+  <si>
+    <t>listbox</t>
   </si>
 </sst>
 </file>
@@ -1001,11 +1019,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:BW3"/>
+  <dimension ref="A1:CC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="BZ7" sqref="BZ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1041,7 @@
     <col min="11" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1249,8 +1267,26 @@
       <c r="BW1" s="7" t="s">
         <v>140</v>
       </c>
+      <c r="BX1" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="BY1" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="BZ1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="CA1" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="CB1" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="CC1" s="7" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1412,8 +1448,14 @@
       <c r="BU2" s="9"/>
       <c r="BV2" s="9"/>
       <c r="BW2" s="9"/>
+      <c r="BX2" s="9"/>
+      <c r="BY2" s="9"/>
+      <c r="BZ2" s="9"/>
+      <c r="CA2" s="9"/>
+      <c r="CB2" s="9"/>
+      <c r="CC2" s="9"/>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -1525,6 +1567,12 @@
       <c r="BU3" s="9"/>
       <c r="BV3" s="9"/>
       <c r="BW3" s="9"/>
+      <c r="BX3" s="9"/>
+      <c r="BY3" s="9"/>
+      <c r="BZ3" s="9"/>
+      <c r="CA3" s="9"/>
+      <c r="CB3" s="9"/>
+      <c r="CC3" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
SMX DP scripting done
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="150">
   <si>
     <t>Environment</t>
   </si>
@@ -463,6 +463,15 @@
   </si>
   <si>
     <t>listbox</t>
+  </si>
+  <si>
+    <t>demographics</t>
+  </si>
+  <si>
+    <t>subquestions</t>
+  </si>
+  <si>
+    <t>symbolratingscale</t>
   </si>
 </sst>
 </file>
@@ -1019,11 +1028,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CC3"/>
+  <dimension ref="A1:CF3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BZ7" sqref="BZ7"/>
+      <selection pane="bottomLeft" activeCell="CD8" sqref="CD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1050,7 @@
     <col min="11" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1285,8 +1294,17 @@
       <c r="CC1" s="7" t="s">
         <v>146</v>
       </c>
+      <c r="CD1" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="CE1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="CF1" s="7" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1454,8 +1472,11 @@
       <c r="CA2" s="9"/>
       <c r="CB2" s="9"/>
       <c r="CC2" s="9"/>
+      <c r="CD2" s="9"/>
+      <c r="CE2" s="9"/>
+      <c r="CF2" s="9"/>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -1573,6 +1594,9 @@
       <c r="CA3" s="9"/>
       <c r="CB3" s="9"/>
       <c r="CC3" s="9"/>
+      <c r="CD3" s="9"/>
+      <c r="CE3" s="9"/>
+      <c r="CF3" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
data added in smx tc and smx dp completed with required maintenance
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -13,6 +13,7 @@
     <sheet name="SanityTC" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="183">
   <si>
     <t>Environment</t>
   </si>
@@ -357,21 +358,12 @@
     <t>Spanish</t>
   </si>
   <si>
-    <t>Please fill the survey and help us improve!</t>
-  </si>
-  <si>
-    <t>Enter your Name</t>
-  </si>
-  <si>
     <t>radiobutton</t>
   </si>
   <si>
     <t>AnswerOptions</t>
   </si>
   <si>
-    <t>Please select the options from the given list</t>
-  </si>
-  <si>
     <t>Endorsement</t>
   </si>
   <si>
@@ -381,9 +373,6 @@
     <t>Please select your choices from the list</t>
   </si>
   <si>
-    <t xml:space="preserve"> Start with a Blank Survey Button not present on page.</t>
-  </si>
-  <si>
     <t>imagechoice</t>
   </si>
   <si>
@@ -472,6 +461,117 @@
   </si>
   <si>
     <t>symbolratingscale</t>
+  </si>
+  <si>
+    <t>How long have you been our customer?</t>
+  </si>
+  <si>
+    <t>How would you rate our company in the following areas?</t>
+  </si>
+  <si>
+    <t>How likely is it that you would recommend our company to a friend or colleague?</t>
+  </si>
+  <si>
+    <t>What are the specific details of the product / service.</t>
+  </si>
+  <si>
+    <t>Where did you last purchase THE PRODUCT?</t>
+  </si>
+  <si>
+    <t>This survey is for manufacturers and product distributors to get a sense of how current and prospective customers responded to a particular product.</t>
+  </si>
+  <si>
+    <t>Please fill below information.</t>
+  </si>
+  <si>
+    <t>For how many years have you been using THE PRODUCT?</t>
+  </si>
+  <si>
+    <t>Would you recommend the product to others?</t>
+  </si>
+  <si>
+    <t>To what extent do you think that THE PRODUCT is worth the price?</t>
+  </si>
+  <si>
+    <t>Where do you usually purchase THE PRODUCT?</t>
+  </si>
+  <si>
+    <t>Please enter the date of birth</t>
+  </si>
+  <si>
+    <t>Where you like to travel from the below place</t>
+  </si>
+  <si>
+    <t>Please enter your qualification details below</t>
+  </si>
+  <si>
+    <t>PHD</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Where do you usually sell the product</t>
+  </si>
+  <si>
+    <t>Intensity</t>
+  </si>
+  <si>
+    <t>Please select all the applicable things you like</t>
+  </si>
+  <si>
+    <t>Rate your skills</t>
+  </si>
+  <si>
+    <t>Rate the importance of things you value</t>
+  </si>
+  <si>
+    <t>Upload your documents</t>
+  </si>
+  <si>
+    <t>What is the highest level of education you completed?</t>
+  </si>
+  <si>
+    <t>Which Product/Service type do you want to provide your feedback about</t>
+  </si>
+  <si>
+    <t>How did you first learn about THE PRODUCT?</t>
+  </si>
+  <si>
+    <t>Are you the principal shopper in your household?</t>
+  </si>
+  <si>
+    <t>The morale in my department is high.</t>
+  </si>
+  <si>
+    <t>Please indicate the extent to which you agree with the following statements.</t>
+  </si>
+  <si>
+    <t>6;7</t>
+  </si>
+  <si>
+    <t>image of mountain.jpg;harley-davidson-logo-vector.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The company clearly conveys its mission to its employees.;There is good communication from managers to employees.;I have the tools and resources I need to do my job. ;I have the training I need to do my job. ;I feel underutilized in my job. ;The amount of work expected of me is reasonable. </t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Do you use THE PRODUCT all of the time or rarely when PERFORMING THE FUNCTION FOR WHICH ITS DESIGNED?</t>
+  </si>
+  <si>
+    <t>AnswerOptions1</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rating Scale Grid Added Do you use THE PRODUCT all of the time or rarely when PERFORMING THE FUNCTION FOR WHICH IT'S DESIGNED? not present on page.</t>
+  </si>
+  <si>
+    <t>PERFORMING THE FUNCTION FOR WHICH ITS DESIGNED?</t>
   </si>
 </sst>
 </file>
@@ -510,7 +610,6 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -533,7 +632,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -589,7 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -601,6 +700,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1028,11 +1128,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CF3"/>
+  <dimension ref="A1:CG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BN1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CD8" sqref="CD8"/>
+      <selection pane="bottomLeft" activeCell="BX3" sqref="BX3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1150,7 @@
     <col min="11" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1205,106 +1305,109 @@
         <v>109</v>
       </c>
       <c r="AZ1" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="BA1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="BC1" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="BB1" s="7" t="s">
+      <c r="BD1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="BE1" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="BC1" s="7" t="s">
+      <c r="BF1" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="BG1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="BH1" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="BD1" s="7" t="s">
+      <c r="BI1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="BE1" s="7" t="s">
+      <c r="BJ1" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="BF1" s="7" t="s">
+      <c r="BK1" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="BG1" s="7" t="s">
+      <c r="BL1" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="BH1" s="7" t="s">
+      <c r="BM1" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="BI1" s="7" t="s">
+      <c r="BN1" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BO1" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="BK1" s="7" t="s">
+      <c r="BP1" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="BL1" s="7" t="s">
+      <c r="BQ1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="BM1" s="7" t="s">
+      <c r="BR1" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="BN1" s="7" t="s">
+      <c r="BS1" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="BO1" s="7" t="s">
+      <c r="BT1" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="BP1" s="7" t="s">
+      <c r="BU1" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="BQ1" s="7" t="s">
+      <c r="BV1" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="BR1" s="7" t="s">
+      <c r="BW1" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="BS1" s="7" t="s">
+      <c r="BX1" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="BT1" s="7" t="s">
+      <c r="BY1" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="BU1" s="7" t="s">
+      <c r="BZ1" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="BV1" s="7" t="s">
+      <c r="CA1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="BW1" s="7" t="s">
+      <c r="CB1" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="BX1" s="7" t="s">
+      <c r="CC1" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="BY1" s="7" t="s">
+      <c r="CD1" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="BZ1" s="7" t="s">
+      <c r="CE1" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="CA1" s="7" t="s">
+      <c r="CF1" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="CB1" s="7" t="s">
+      <c r="CG1" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="CC1" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="CD1" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="CE1" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="CF1" s="7" t="s">
-        <v>149</v>
-      </c>
     </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1475,8 +1578,9 @@
       <c r="CD2" s="9"/>
       <c r="CE2" s="9"/>
       <c r="CF2" s="9"/>
+      <c r="CG2" s="9"/>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -1499,11 +1603,11 @@
       <c r="H3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>38</v>
+      <c r="I3" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>119</v>
+        <v>181</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="2"/>
@@ -1553,50 +1657,113 @@
         <v>110</v>
       </c>
       <c r="AX3" s="9" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="AY3" s="9" t="s">
-        <v>112</v>
+        <v>149</v>
       </c>
       <c r="AZ3" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA3" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB3" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="BC3" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="BA3" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="BB3" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="BC3" s="9"/>
-      <c r="BD3" s="9"/>
-      <c r="BE3" s="9"/>
-      <c r="BF3" s="9"/>
-      <c r="BG3" s="9"/>
-      <c r="BH3" s="9"/>
-      <c r="BI3" s="9"/>
-      <c r="BJ3" s="9"/>
-      <c r="BK3" s="9"/>
-      <c r="BL3" s="9"/>
-      <c r="BM3" s="9"/>
-      <c r="BN3" s="9"/>
-      <c r="BO3" s="9"/>
-      <c r="BP3" s="9"/>
-      <c r="BQ3" s="9"/>
-      <c r="BR3" s="9"/>
-      <c r="BS3" s="9"/>
-      <c r="BT3" s="9"/>
-      <c r="BU3" s="9"/>
-      <c r="BV3" s="9"/>
-      <c r="BW3" s="9"/>
-      <c r="BX3" s="9"/>
-      <c r="BY3" s="9"/>
-      <c r="BZ3" s="9"/>
-      <c r="CA3" s="9"/>
-      <c r="CB3" s="9"/>
-      <c r="CC3" s="9"/>
-      <c r="CD3" s="9"/>
-      <c r="CE3" s="9"/>
-      <c r="CF3" s="9"/>
+      <c r="BD3" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="BE3" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="BF3" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="BG3" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="BH3" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="BI3" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="BJ3" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK3" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL3" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM3" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN3" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO3" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP3" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="BQ3" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="BR3" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS3" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="BT3" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="BU3" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BV3" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BW3" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="BX3" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BY3" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ3" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="CA3" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="CB3" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="CC3" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="CD3" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="CE3" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="CF3" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="CG3" s="9" t="s">
+        <v>173</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
conflicts resolved in excl file and tc file
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -13,9 +13,8 @@
     <sheet name="SanityTC" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="188">
   <si>
     <t>Environment</t>
   </si>
@@ -556,9 +555,6 @@
     <t xml:space="preserve">The company clearly conveys its mission to its employees.;There is good communication from managers to employees.;I have the tools and resources I need to do my job. ;I have the training I need to do my job. ;I feel underutilized in my job. ;The amount of work expected of me is reasonable. </t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>Do you use THE PRODUCT all of the time or rarely when PERFORMING THE FUNCTION FOR WHICH ITS DESIGNED?</t>
   </si>
   <si>
@@ -568,27 +564,35 @@
     <t>Qualification</t>
   </si>
   <si>
-    <t xml:space="preserve"> Rating Scale Grid Added Do you use THE PRODUCT all of the time or rarely when PERFORMING THE FUNCTION FOR WHICH IT'S DESIGNED? not present on page.</t>
-  </si>
-  <si>
     <t>PERFORMING THE FUNCTION FOR WHICH ITS DESIGNED?</t>
   </si>
   <si>
-    <t xml:space="preserve"> Like/Dislike Added Do you use THE PRODUCT all of the time or rarely when PERFORMING THE FUNCTION FOR WHICH ITS DESIGNED? not present on page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Use this list Button not present on page.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Loader did not disappear.</t>
+  </si>
+  <si>
+    <t>Sanity_TC3</t>
+  </si>
+  <si>
+    <t>Sanity_TC4</t>
+  </si>
+  <si>
+    <t>Sanity_TC5</t>
+  </si>
+  <si>
+    <t>Sanity_TC8</t>
+  </si>
+  <si>
+    <t>Sanity_TC9</t>
+  </si>
+  <si>
+    <t>Sanity_TC10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,62 +626,12 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -697,156 +651,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="13"/>
       </patternFill>
     </fill>
@@ -903,7 +712,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -916,27 +725,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1227,8 +1020,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1271,9 +1064,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1318,10 +1111,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1363,26 +1156,26 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CG3"/>
+  <dimension ref="A1:CG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BX3" sqref="BX3"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="11" max="13" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:85" x14ac:dyDescent="0.25">
@@ -1546,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="BB1" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BC1" s="7" t="s">
         <v>114</v>
@@ -1838,11 +1631,11 @@
       <c r="H3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="12" t="s">
         <v>38</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="2"/>
@@ -1904,7 +1697,7 @@
         <v>113</v>
       </c>
       <c r="BB3" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="BC3" s="9" t="s">
         <v>115</v>
@@ -1922,7 +1715,7 @@
         <v>157</v>
       </c>
       <c r="BH3" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="BI3" s="9" t="s">
         <v>148</v>
@@ -1967,7 +1760,7 @@
         <v>166</v>
       </c>
       <c r="BW3" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="BX3" s="9" t="s">
         <v>168</v>
@@ -1997,6 +1790,1116 @@
         <v>176</v>
       </c>
       <c r="CG3" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="9"/>
+      <c r="AP4" s="9"/>
+      <c r="AQ4" s="9"/>
+      <c r="AR4" s="9"/>
+      <c r="AS4" s="9"/>
+      <c r="AT4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV4" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW4" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX4" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ4" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB4" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="BC4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="BD4" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="BE4" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="BF4" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="BG4" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="BH4" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI4" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="BJ4" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK4" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL4" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM4" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN4" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO4" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP4" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="BQ4" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="BR4" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS4" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="BT4" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="BU4" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BV4" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BW4" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="BX4" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BY4" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ4" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="CA4" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="CB4" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="CC4" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="CD4" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="CE4" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="CF4" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="CG4" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="9"/>
+      <c r="AP5" s="9"/>
+      <c r="AQ5" s="9"/>
+      <c r="AR5" s="9"/>
+      <c r="AS5" s="9"/>
+      <c r="AT5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX5" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY5" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ5" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB5" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="BC5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="BD5" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="BE5" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="BF5" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="BG5" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="BH5" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI5" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="BJ5" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK5" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL5" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM5" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN5" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO5" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP5" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="BQ5" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="BR5" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS5" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="BT5" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="BU5" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BV5" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BW5" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="BX5" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BY5" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ5" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="CA5" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="CB5" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="CC5" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="CD5" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="CE5" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="CF5" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="CG5" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="6"/>
+      <c r="AM6" s="6"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU6" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV6" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW6" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX6" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY6" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ6" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA6" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB6" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="BC6" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="BD6" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="BE6" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="BF6" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="BG6" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="BH6" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI6" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="BJ6" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK6" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL6" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM6" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN6" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO6" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP6" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="BQ6" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="BR6" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS6" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="BT6" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="BU6" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BV6" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BW6" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="BX6" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BY6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ6" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="CA6" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="CB6" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="CC6" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="CD6" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="CE6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="CF6" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="CG6" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="15"/>
+      <c r="AP7" s="15"/>
+      <c r="AQ7" s="15"/>
+      <c r="AR7" s="15"/>
+      <c r="AS7" s="15"/>
+      <c r="AT7" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU7" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV7" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW7" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX7" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY7" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ7" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA7" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB7" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="BC7" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="BD7" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="BE7" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="BF7" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="BG7" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="BH7" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI7" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="BJ7" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK7" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL7" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM7" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN7" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO7" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP7" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="BQ7" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="BR7" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS7" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="BT7" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="BU7" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="BV7" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="BW7" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="BX7" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="BY7" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ7" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="CA7" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="CB7" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="CC7" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="CD7" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="CE7" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CF7" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="CG7" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="15"/>
+      <c r="AP8" s="15"/>
+      <c r="AQ8" s="15"/>
+      <c r="AR8" s="15"/>
+      <c r="AS8" s="15"/>
+      <c r="AT8" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU8" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV8" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW8" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX8" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY8" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ8" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA8" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB8" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="BC8" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="BD8" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="BE8" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="BF8" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="BG8" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="BH8" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI8" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="BJ8" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK8" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL8" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM8" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN8" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO8" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP8" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="BQ8" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="BR8" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS8" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="BT8" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="BU8" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="BV8" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="BW8" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="BX8" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="BY8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ8" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="CA8" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="CB8" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="CC8" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="CD8" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="CE8" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CF8" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="CG8" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="6"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="15"/>
+      <c r="AP9" s="15"/>
+      <c r="AQ9" s="15"/>
+      <c r="AR9" s="15"/>
+      <c r="AS9" s="15"/>
+      <c r="AT9" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU9" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV9" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW9" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX9" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY9" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ9" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA9" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB9" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="BC9" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="BD9" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="BE9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="BF9" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="BG9" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="BH9" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI9" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="BJ9" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK9" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL9" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM9" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN9" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO9" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP9" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="BQ9" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="BR9" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS9" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="BT9" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="BU9" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="BV9" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="BW9" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="BX9" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="BY9" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ9" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="CA9" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="CB9" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="CC9" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="CD9" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="CE9" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CF9" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="CG9" s="15" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dmx less than 1000
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="206">
   <si>
     <t>Environment</t>
   </si>
@@ -567,33 +567,86 @@
     <t>Sanity_TC3</t>
   </si>
   <si>
-    <t>Create DMX survey</t>
-  </si>
-  <si>
     <t>survey should be distributed</t>
   </si>
   <si>
     <t>surveyid</t>
   </si>
   <si>
-    <t>5430</t>
-  </si>
-  <si>
-    <t>DP test yellow jacket</t>
-  </si>
-  <si>
     <t>emailtemplate</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DMX</t>
+  </si>
+  <si>
+    <t>sogo_suhayl</t>
+  </si>
+  <si>
+    <t>Canopus4sogosurvey</t>
+  </si>
+  <si>
+    <t>282</t>
+  </si>
+  <si>
+    <t>INVITE DMX EXE DP</t>
+  </si>
+  <si>
+    <t>1010 NEW DMX DP EXE LIST [1010 records]</t>
+  </si>
+  <si>
+    <t>selectlist</t>
+  </si>
+  <si>
+    <t>mailmergedd</t>
+  </si>
+  <si>
+    <t>Salutation;Gender;Last Name</t>
+  </si>
+  <si>
+    <t>mailmergetxt</t>
+  </si>
+  <si>
+    <t>Mr;Male;Tandel</t>
+  </si>
+  <si>
+    <t>prepopdd</t>
+  </si>
+  <si>
+    <t>Salutation</t>
+  </si>
+  <si>
+    <t>Sanity_TC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To send exe invite </t>
+  </si>
+  <si>
+    <t>To send Platfrom Invite &amp; PF reminder</t>
+  </si>
+  <si>
+    <t>283</t>
+  </si>
+  <si>
+    <t>PALTROMINV DMX DP</t>
+  </si>
+  <si>
+    <t>New DMX DP PF SOGO [16 records]</t>
+  </si>
+  <si>
+    <t>emailtemplatere</t>
+  </si>
+  <si>
+    <t>Reminder_EXE DP RA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,31 +678,16 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,66 +708,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
       </patternFill>
     </fill>
   </fills>
@@ -785,7 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -799,14 +777,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1097,8 +1068,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,9 +1112,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1180,18 +1151,18 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,6 +1190,20 @@
         <v>96</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1227,35 +1212,36 @@
     <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CI4"/>
+  <dimension ref="A1:CN5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BM1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BS1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CI4" sqref="CI4"/>
+      <selection pane="bottomLeft" activeCell="CL9" sqref="CL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="11" max="13" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1512,13 +1498,28 @@
         <v>144</v>
       </c>
       <c r="CH1" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="CI1" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="CI1" s="7" t="s">
-        <v>186</v>
+      <c r="CJ1" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="CK1" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="CL1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="CM1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="CN1" s="7" t="s">
+        <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1690,8 +1691,13 @@
       <c r="CG2" s="9"/>
       <c r="CH2" s="9"/>
       <c r="CI2" s="9"/>
+      <c r="CJ2" s="9"/>
+      <c r="CK2" s="9"/>
+      <c r="CL2" s="9"/>
+      <c r="CM2" s="9"/>
+      <c r="CN2" s="9"/>
     </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -1875,8 +1881,13 @@
       </c>
       <c r="CH3" s="9"/>
       <c r="CI3" s="9"/>
+      <c r="CJ3" s="9"/>
+      <c r="CK3" s="9"/>
+      <c r="CL3" s="9"/>
+      <c r="CM3" s="9"/>
+      <c r="CN3" s="9"/>
     </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>180</v>
       </c>
@@ -1890,18 +1901,16 @@
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>185</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>187</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="I4" s="13"/>
       <c r="J4" s="2"/>
       <c r="K4" s="1"/>
       <c r="L4" s="2"/>
@@ -1938,131 +1947,188 @@
       <c r="AQ4" s="9"/>
       <c r="AR4" s="9"/>
       <c r="AS4" s="9"/>
-      <c r="AT4" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AU4" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV4" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AW4" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="AX4" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="AY4" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="AZ4" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="BA4" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="BB4" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="BC4" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="BD4" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="BE4" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="BF4" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="BG4" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="BH4" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="BI4" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="BJ4" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="BK4" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="BL4" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="BM4" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="BN4" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="BO4" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="BP4" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="BQ4" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="BR4" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="BS4" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="BT4" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="BU4" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="BV4" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="BW4" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="BX4" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="BY4" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="BZ4" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="CA4" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="CB4" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="CC4" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="CD4" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="CE4" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="CF4" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="CG4" s="9" t="s">
-        <v>172</v>
-      </c>
+      <c r="AT4" s="9"/>
+      <c r="AU4" s="9"/>
+      <c r="AV4" s="9"/>
+      <c r="AW4" s="9"/>
+      <c r="AX4" s="9"/>
+      <c r="AY4" s="9"/>
+      <c r="AZ4" s="9"/>
+      <c r="BA4" s="9"/>
+      <c r="BB4" s="9"/>
+      <c r="BC4" s="9"/>
+      <c r="BD4" s="9"/>
+      <c r="BE4" s="11"/>
+      <c r="BF4" s="9"/>
+      <c r="BG4" s="9"/>
+      <c r="BH4" s="9"/>
+      <c r="BI4" s="9"/>
+      <c r="BJ4" s="9"/>
+      <c r="BK4" s="9"/>
+      <c r="BL4" s="9"/>
+      <c r="BM4" s="9"/>
+      <c r="BN4" s="9"/>
+      <c r="BO4" s="9"/>
+      <c r="BP4" s="9"/>
+      <c r="BQ4" s="9"/>
+      <c r="BR4" s="9"/>
+      <c r="BS4" s="9"/>
+      <c r="BT4" s="9"/>
+      <c r="BU4" s="9"/>
+      <c r="BV4" s="9"/>
+      <c r="BW4" s="9"/>
+      <c r="BX4" s="9"/>
+      <c r="BY4" s="9"/>
+      <c r="BZ4" s="9"/>
+      <c r="CA4" s="9"/>
+      <c r="CB4" s="9"/>
+      <c r="CC4" s="9"/>
+      <c r="CD4" s="9"/>
+      <c r="CE4" s="9"/>
+      <c r="CF4" s="9"/>
+      <c r="CG4" s="9"/>
       <c r="CH4" s="11" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="CI4" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="CJ4" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="CK4" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="CL4" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="CM4" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="CN4" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>185</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="9"/>
+      <c r="AP5" s="9"/>
+      <c r="AQ5" s="9"/>
+      <c r="AR5" s="9"/>
+      <c r="AS5" s="9"/>
+      <c r="AT5" s="9"/>
+      <c r="AU5" s="9"/>
+      <c r="AV5" s="9"/>
+      <c r="AW5" s="9"/>
+      <c r="AX5" s="9"/>
+      <c r="AY5" s="9"/>
+      <c r="AZ5" s="9"/>
+      <c r="BA5" s="9"/>
+      <c r="BB5" s="9"/>
+      <c r="BC5" s="9"/>
+      <c r="BD5" s="9"/>
+      <c r="BE5" s="11"/>
+      <c r="BF5" s="9"/>
+      <c r="BG5" s="9"/>
+      <c r="BH5" s="9"/>
+      <c r="BI5" s="9"/>
+      <c r="BJ5" s="9"/>
+      <c r="BK5" s="9"/>
+      <c r="BL5" s="9"/>
+      <c r="BM5" s="9"/>
+      <c r="BN5" s="9"/>
+      <c r="BO5" s="9"/>
+      <c r="BP5" s="9"/>
+      <c r="BQ5" s="9"/>
+      <c r="BR5" s="9"/>
+      <c r="BS5" s="9"/>
+      <c r="BT5" s="9"/>
+      <c r="BU5" s="9"/>
+      <c r="BV5" s="9"/>
+      <c r="BW5" s="9"/>
+      <c r="BX5" s="9"/>
+      <c r="BY5" s="9"/>
+      <c r="BZ5" s="9"/>
+      <c r="CA5" s="9"/>
+      <c r="CB5" s="9"/>
+      <c r="CC5" s="9"/>
+      <c r="CD5" s="9"/>
+      <c r="CE5" s="9"/>
+      <c r="CF5" s="9"/>
+      <c r="CG5" s="9"/>
+      <c r="CH5" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="CI5" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="CJ5" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="CK5" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="CL5" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="CM5" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="CN5" s="11" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dmx dp cases added
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="216">
   <si>
     <t>Environment</t>
   </si>
@@ -640,6 +640,36 @@
   </si>
   <si>
     <t>Reminder_EXE DP RA</t>
+  </si>
+  <si>
+    <t>Sanity_TC5</t>
+  </si>
+  <si>
+    <t>SMS numbers.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send SMS invites and reminder </t>
+  </si>
+  <si>
+    <t>Sanity_TC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downloading SAP </t>
+  </si>
+  <si>
+    <t>survey should be downloaded</t>
+  </si>
+  <si>
+    <t>Contact list DP.xlsx</t>
+  </si>
+  <si>
+    <t>Email Address;Status;First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create new list </t>
+  </si>
+  <si>
+    <t>Sanity_TC7</t>
   </si>
 </sst>
 </file>
@@ -763,7 +793,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -778,6 +808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1219,11 +1250,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CN5"/>
+  <dimension ref="A1:CN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BS1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CL9" sqref="CL9"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2131,6 +2162,346 @@
         <v>202</v>
       </c>
     </row>
+    <row r="6" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="6"/>
+      <c r="AM6" s="6"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="9"/>
+      <c r="AX6" s="9"/>
+      <c r="AY6" s="9"/>
+      <c r="AZ6" s="9"/>
+      <c r="BA6" s="9"/>
+      <c r="BB6" s="9"/>
+      <c r="BC6" s="9"/>
+      <c r="BD6" s="9"/>
+      <c r="BE6" s="11"/>
+      <c r="BF6" s="9"/>
+      <c r="BG6" s="9"/>
+      <c r="BH6" s="9"/>
+      <c r="BI6" s="9"/>
+      <c r="BJ6" s="9"/>
+      <c r="BK6" s="9"/>
+      <c r="BL6" s="9"/>
+      <c r="BM6" s="9"/>
+      <c r="BN6" s="9"/>
+      <c r="BO6" s="9"/>
+      <c r="BP6" s="9"/>
+      <c r="BQ6" s="9"/>
+      <c r="BR6" s="9"/>
+      <c r="BS6" s="9"/>
+      <c r="BT6" s="9"/>
+      <c r="BU6" s="9"/>
+      <c r="BV6" s="9"/>
+      <c r="BW6" s="9"/>
+      <c r="BX6" s="9"/>
+      <c r="BY6" s="9"/>
+      <c r="BZ6" s="9"/>
+      <c r="CA6" s="9"/>
+      <c r="CB6" s="9"/>
+      <c r="CC6" s="9"/>
+      <c r="CD6" s="9"/>
+      <c r="CE6" s="9"/>
+      <c r="CF6" s="9"/>
+      <c r="CG6" s="9"/>
+      <c r="CH6" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="CI6" s="11"/>
+      <c r="CJ6" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="CK6" s="11"/>
+      <c r="CL6" s="11"/>
+      <c r="CM6" s="11"/>
+      <c r="CN6" s="11"/>
+    </row>
+    <row r="7" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="9"/>
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="9"/>
+      <c r="AW7" s="9"/>
+      <c r="AX7" s="9"/>
+      <c r="AY7" s="9"/>
+      <c r="AZ7" s="9"/>
+      <c r="BA7" s="9"/>
+      <c r="BB7" s="9"/>
+      <c r="BC7" s="9"/>
+      <c r="BD7" s="9"/>
+      <c r="BE7" s="11"/>
+      <c r="BF7" s="9"/>
+      <c r="BG7" s="9"/>
+      <c r="BH7" s="9"/>
+      <c r="BI7" s="9"/>
+      <c r="BJ7" s="9"/>
+      <c r="BK7" s="9"/>
+      <c r="BL7" s="9"/>
+      <c r="BM7" s="9"/>
+      <c r="BN7" s="9"/>
+      <c r="BO7" s="9"/>
+      <c r="BP7" s="9"/>
+      <c r="BQ7" s="9"/>
+      <c r="BR7" s="9"/>
+      <c r="BS7" s="9"/>
+      <c r="BT7" s="9"/>
+      <c r="BU7" s="9"/>
+      <c r="BV7" s="9"/>
+      <c r="BW7" s="9"/>
+      <c r="BX7" s="9"/>
+      <c r="BY7" s="9"/>
+      <c r="BZ7" s="9"/>
+      <c r="CA7" s="9"/>
+      <c r="CB7" s="9"/>
+      <c r="CC7" s="9"/>
+      <c r="CD7" s="9"/>
+      <c r="CE7" s="9"/>
+      <c r="CF7" s="9"/>
+      <c r="CG7" s="9"/>
+      <c r="CH7" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="CI7" s="11"/>
+      <c r="CJ7" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="CK7" s="11"/>
+      <c r="CL7" s="11"/>
+      <c r="CM7" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="CN7" s="11"/>
+    </row>
+    <row r="8" spans="1:92" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="9"/>
+      <c r="AS8" s="9"/>
+      <c r="AT8" s="9"/>
+      <c r="AU8" s="9"/>
+      <c r="AV8" s="9"/>
+      <c r="AW8" s="9"/>
+      <c r="AX8" s="9"/>
+      <c r="AY8" s="9"/>
+      <c r="AZ8" s="9"/>
+      <c r="BA8" s="9"/>
+      <c r="BB8" s="9"/>
+      <c r="BC8" s="9"/>
+      <c r="BD8" s="9"/>
+      <c r="BE8" s="11"/>
+      <c r="BF8" s="9"/>
+      <c r="BG8" s="9"/>
+      <c r="BH8" s="9"/>
+      <c r="BI8" s="9"/>
+      <c r="BJ8" s="9"/>
+      <c r="BK8" s="9"/>
+      <c r="BL8" s="9"/>
+      <c r="BM8" s="9"/>
+      <c r="BN8" s="9"/>
+      <c r="BO8" s="9"/>
+      <c r="BP8" s="9"/>
+      <c r="BQ8" s="9"/>
+      <c r="BR8" s="9"/>
+      <c r="BS8" s="9"/>
+      <c r="BT8" s="9"/>
+      <c r="BU8" s="9"/>
+      <c r="BV8" s="9"/>
+      <c r="BW8" s="9"/>
+      <c r="BX8" s="9"/>
+      <c r="BY8" s="9"/>
+      <c r="BZ8" s="9"/>
+      <c r="CA8" s="9"/>
+      <c r="CB8" s="9"/>
+      <c r="CC8" s="9"/>
+      <c r="CD8" s="9"/>
+      <c r="CE8" s="9"/>
+      <c r="CF8" s="9"/>
+      <c r="CG8" s="9"/>
+      <c r="CH8" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="CI8" s="11"/>
+      <c r="CJ8" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="CK8" s="11"/>
+      <c r="CL8" s="11"/>
+      <c r="CM8" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="CN8" s="11"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="W2" r:id="rId1" display="test3t@aiktefs.com"/>

</xml_diff>

<commit_message>
K12 Nightsupport readings done and have written code in Engage Sanity for code reusebility
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3357B7D2-D57D-478A-8B07-07BDDA18AA72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="210">
   <si>
     <t>Environment</t>
   </si>
@@ -640,13 +641,26 @@
   </si>
   <si>
     <t>Reminder_EXE DP RA</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sogo Account not present on page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 05 not present on page.</t>
+  </si>
+  <si>
+    <t>SKIP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,16 +692,53 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
+    </font>
+    <font>
       <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -707,7 +758,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
   </fills>
@@ -763,7 +934,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -774,10 +945,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1058,7 +1245,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1068,8 +1255,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1096,14 +1283,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.google.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.google.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1112,9 +1299,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,7 +1328,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1149,7 +1336,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1159,10 +1346,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1209,7 +1396,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019"/>
+    <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1217,28 +1404,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CN5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BS1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CL9" sqref="CL9"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="11" max="13" customWidth="true" width="32.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:92" x14ac:dyDescent="0.25">
@@ -1524,7 +1711,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -1542,8 +1729,8 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>37</v>
+      <c r="I2" s="28" t="s">
+        <v>209</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
@@ -1702,7 +1889,7 @@
         <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -1720,10 +1907,12 @@
       <c r="H3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="2"/>
+      <c r="I3" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>207</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1792,7 +1981,7 @@
       <c r="BD3" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="BE3" s="11" t="s">
+      <c r="BE3" s="10" t="s">
         <v>173</v>
       </c>
       <c r="BF3" s="9" t="s">
@@ -1892,7 +2081,7 @@
         <v>180</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -1910,8 +2099,12 @@
       <c r="H4" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="2"/>
+      <c r="I4" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>208</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1958,7 +2151,7 @@
       <c r="BB4" s="9"/>
       <c r="BC4" s="9"/>
       <c r="BD4" s="9"/>
-      <c r="BE4" s="11"/>
+      <c r="BE4" s="10"/>
       <c r="BF4" s="9"/>
       <c r="BG4" s="9"/>
       <c r="BH4" s="9"/>
@@ -1987,25 +2180,25 @@
       <c r="CE4" s="9"/>
       <c r="CF4" s="9"/>
       <c r="CG4" s="9"/>
-      <c r="CH4" s="11" t="s">
+      <c r="CH4" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="CI4" s="11" t="s">
+      <c r="CI4" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="CJ4" s="11" t="s">
+      <c r="CJ4" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="CK4" s="11" t="s">
+      <c r="CK4" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="CL4" s="11" t="s">
+      <c r="CL4" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="CM4" s="11" t="s">
+      <c r="CM4" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="CN4" s="11" t="s">
+      <c r="CN4" s="10" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2014,7 +2207,7 @@
         <v>198</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -2032,7 +2225,9 @@
       <c r="H5" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="I5" s="13"/>
+      <c r="I5" s="28" t="s">
+        <v>209</v>
+      </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
       <c r="L5" s="2"/>
@@ -2080,7 +2275,7 @@
       <c r="BB5" s="9"/>
       <c r="BC5" s="9"/>
       <c r="BD5" s="9"/>
-      <c r="BE5" s="11"/>
+      <c r="BE5" s="10"/>
       <c r="BF5" s="9"/>
       <c r="BG5" s="9"/>
       <c r="BH5" s="9"/>
@@ -2109,31 +2304,31 @@
       <c r="CE5" s="9"/>
       <c r="CF5" s="9"/>
       <c r="CG5" s="9"/>
-      <c r="CH5" s="11" t="s">
+      <c r="CH5" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="CI5" s="11" t="s">
+      <c r="CI5" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="CJ5" s="11" t="s">
+      <c r="CJ5" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="CK5" s="11" t="s">
+      <c r="CK5" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="CL5" s="11" t="s">
+      <c r="CL5" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="CM5" s="11" t="s">
+      <c r="CM5" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="CN5" s="11" t="s">
+      <c r="CN5" s="10" t="s">
         <v>202</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W2" r:id="rId1" display="test3t@aiktefs.com"/>
+    <hyperlink ref="W2" r:id="rId1" display="test3t@aiktefs.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
sogo and k12 smoke suite created with smx dp
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA32E40E-D021-4767-8FA0-477F8BDBA3D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="218">
   <si>
     <t>Environment</t>
   </si>
@@ -682,7 +681,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1130,7 +1129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1168,14 +1167,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.google.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.google.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1213,7 +1212,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1221,7 +1220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1281,7 +1280,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1289,13 +1288,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,7 +1595,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>183</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -1792,7 +1791,7 @@
       <c r="H3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="18" t="s">
         <v>207</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1984,7 +1983,7 @@
       <c r="H4" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="18" t="s">
         <v>207</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -2110,7 +2109,7 @@
       <c r="H5" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="18" t="s">
         <v>207</v>
       </c>
       <c r="J5" s="2"/>
@@ -2216,7 +2215,7 @@
         <v>208</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -2234,7 +2233,9 @@
       <c r="H6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I6" s="12"/>
+      <c r="I6" s="18" t="s">
+        <v>207</v>
+      </c>
       <c r="J6" s="13"/>
       <c r="K6" s="1"/>
       <c r="L6" s="13"/>
@@ -2328,7 +2329,7 @@
         <v>211</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -2346,7 +2347,9 @@
       <c r="H7" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I7" s="12"/>
+      <c r="I7" s="18" t="s">
+        <v>207</v>
+      </c>
       <c r="J7" s="13"/>
       <c r="K7" s="1"/>
       <c r="L7" s="13"/>
@@ -2442,7 +2445,7 @@
         <v>214</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -2460,7 +2463,9 @@
       <c r="H8" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I8" s="12"/>
+      <c r="I8" s="18" t="s">
+        <v>207</v>
+      </c>
       <c r="J8" s="13"/>
       <c r="K8" s="1"/>
       <c r="L8" s="13"/>
@@ -2553,7 +2558,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W2" r:id="rId1" display="test3t@aiktefs.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="W2" r:id="rId1" display="test3t@aiktefs.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
dmx dp added for engage and research partially
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="220">
   <si>
     <t>Environment</t>
   </si>
@@ -676,6 +676,12 @@
   </si>
   <si>
     <t>Email Address;Status;First Name</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -683,7 +689,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -711,6 +717,22 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -722,7 +744,7 @@
       <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -733,6 +755,41 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
@@ -828,7 +885,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -841,14 +898,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1294,7 +1355,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,7 +1656,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -1613,7 +1674,7 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="22" t="s">
         <v>207</v>
       </c>
       <c r="J2" s="2"/>
@@ -1773,7 +1834,7 @@
         <v>96</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>183</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -1791,8 +1852,8 @@
       <c r="H3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>207</v>
+      <c r="I3" s="20" t="s">
+        <v>219</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>205</v>
@@ -1983,7 +2044,7 @@
       <c r="H4" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="22" t="s">
         <v>207</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -2109,7 +2170,7 @@
       <c r="H5" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="22" t="s">
         <v>207</v>
       </c>
       <c r="J5" s="2"/>
@@ -2233,13 +2294,13 @@
       <c r="H6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="J6" s="13"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -2267,62 +2328,62 @@
       <c r="AL6" s="6"/>
       <c r="AM6" s="6"/>
       <c r="AN6" s="1"/>
-      <c r="AO6" s="14"/>
-      <c r="AP6" s="14"/>
-      <c r="AQ6" s="14"/>
-      <c r="AR6" s="14"/>
-      <c r="AS6" s="14"/>
-      <c r="AT6" s="14"/>
-      <c r="AU6" s="14"/>
-      <c r="AV6" s="14"/>
-      <c r="AW6" s="14"/>
-      <c r="AX6" s="14"/>
-      <c r="AY6" s="14"/>
-      <c r="AZ6" s="14"/>
-      <c r="BA6" s="14"/>
-      <c r="BB6" s="14"/>
-      <c r="BC6" s="14"/>
-      <c r="BD6" s="14"/>
-      <c r="BE6" s="15"/>
-      <c r="BF6" s="14"/>
-      <c r="BG6" s="14"/>
-      <c r="BH6" s="14"/>
-      <c r="BI6" s="14"/>
-      <c r="BJ6" s="14"/>
-      <c r="BK6" s="14"/>
-      <c r="BL6" s="14"/>
-      <c r="BM6" s="14"/>
-      <c r="BN6" s="14"/>
-      <c r="BO6" s="14"/>
-      <c r="BP6" s="14"/>
-      <c r="BQ6" s="14"/>
-      <c r="BR6" s="14"/>
-      <c r="BS6" s="14"/>
-      <c r="BT6" s="14"/>
-      <c r="BU6" s="14"/>
-      <c r="BV6" s="14"/>
-      <c r="BW6" s="14"/>
-      <c r="BX6" s="14"/>
-      <c r="BY6" s="14"/>
-      <c r="BZ6" s="14"/>
-      <c r="CA6" s="14"/>
-      <c r="CB6" s="14"/>
-      <c r="CC6" s="14"/>
-      <c r="CD6" s="14"/>
-      <c r="CE6" s="14"/>
-      <c r="CF6" s="14"/>
-      <c r="CG6" s="14"/>
-      <c r="CH6" s="15" t="s">
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+      <c r="AX6" s="13"/>
+      <c r="AY6" s="13"/>
+      <c r="AZ6" s="13"/>
+      <c r="BA6" s="13"/>
+      <c r="BB6" s="13"/>
+      <c r="BC6" s="13"/>
+      <c r="BD6" s="13"/>
+      <c r="BE6" s="14"/>
+      <c r="BF6" s="13"/>
+      <c r="BG6" s="13"/>
+      <c r="BH6" s="13"/>
+      <c r="BI6" s="13"/>
+      <c r="BJ6" s="13"/>
+      <c r="BK6" s="13"/>
+      <c r="BL6" s="13"/>
+      <c r="BM6" s="13"/>
+      <c r="BN6" s="13"/>
+      <c r="BO6" s="13"/>
+      <c r="BP6" s="13"/>
+      <c r="BQ6" s="13"/>
+      <c r="BR6" s="13"/>
+      <c r="BS6" s="13"/>
+      <c r="BT6" s="13"/>
+      <c r="BU6" s="13"/>
+      <c r="BV6" s="13"/>
+      <c r="BW6" s="13"/>
+      <c r="BX6" s="13"/>
+      <c r="BY6" s="13"/>
+      <c r="BZ6" s="13"/>
+      <c r="CA6" s="13"/>
+      <c r="CB6" s="13"/>
+      <c r="CC6" s="13"/>
+      <c r="CD6" s="13"/>
+      <c r="CE6" s="13"/>
+      <c r="CF6" s="13"/>
+      <c r="CG6" s="13"/>
+      <c r="CH6" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="CI6" s="15"/>
-      <c r="CJ6" s="15" t="s">
+      <c r="CI6" s="14"/>
+      <c r="CJ6" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="CK6" s="15"/>
-      <c r="CL6" s="15"/>
-      <c r="CM6" s="15"/>
-      <c r="CN6" s="15"/>
+      <c r="CK6" s="14"/>
+      <c r="CL6" s="14"/>
+      <c r="CM6" s="14"/>
+      <c r="CN6" s="14"/>
     </row>
     <row r="7" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2347,13 +2408,13 @@
       <c r="H7" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="J7" s="13"/>
+      <c r="J7" s="12"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -2381,64 +2442,64 @@
       <c r="AL7" s="6"/>
       <c r="AM7" s="6"/>
       <c r="AN7" s="1"/>
-      <c r="AO7" s="14"/>
-      <c r="AP7" s="14"/>
-      <c r="AQ7" s="14"/>
-      <c r="AR7" s="14"/>
-      <c r="AS7" s="14"/>
-      <c r="AT7" s="14"/>
-      <c r="AU7" s="14"/>
-      <c r="AV7" s="14"/>
-      <c r="AW7" s="14"/>
-      <c r="AX7" s="14"/>
-      <c r="AY7" s="14"/>
-      <c r="AZ7" s="14"/>
-      <c r="BA7" s="14"/>
-      <c r="BB7" s="14"/>
-      <c r="BC7" s="14"/>
-      <c r="BD7" s="14"/>
-      <c r="BE7" s="15"/>
-      <c r="BF7" s="14"/>
-      <c r="BG7" s="14"/>
-      <c r="BH7" s="14"/>
-      <c r="BI7" s="14"/>
-      <c r="BJ7" s="14"/>
-      <c r="BK7" s="14"/>
-      <c r="BL7" s="14"/>
-      <c r="BM7" s="14"/>
-      <c r="BN7" s="14"/>
-      <c r="BO7" s="14"/>
-      <c r="BP7" s="14"/>
-      <c r="BQ7" s="14"/>
-      <c r="BR7" s="14"/>
-      <c r="BS7" s="14"/>
-      <c r="BT7" s="14"/>
-      <c r="BU7" s="14"/>
-      <c r="BV7" s="14"/>
-      <c r="BW7" s="14"/>
-      <c r="BX7" s="14"/>
-      <c r="BY7" s="14"/>
-      <c r="BZ7" s="14"/>
-      <c r="CA7" s="14"/>
-      <c r="CB7" s="14"/>
-      <c r="CC7" s="14"/>
-      <c r="CD7" s="14"/>
-      <c r="CE7" s="14"/>
-      <c r="CF7" s="14"/>
-      <c r="CG7" s="14"/>
-      <c r="CH7" s="15" t="s">
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+      <c r="AX7" s="13"/>
+      <c r="AY7" s="13"/>
+      <c r="AZ7" s="13"/>
+      <c r="BA7" s="13"/>
+      <c r="BB7" s="13"/>
+      <c r="BC7" s="13"/>
+      <c r="BD7" s="13"/>
+      <c r="BE7" s="14"/>
+      <c r="BF7" s="13"/>
+      <c r="BG7" s="13"/>
+      <c r="BH7" s="13"/>
+      <c r="BI7" s="13"/>
+      <c r="BJ7" s="13"/>
+      <c r="BK7" s="13"/>
+      <c r="BL7" s="13"/>
+      <c r="BM7" s="13"/>
+      <c r="BN7" s="13"/>
+      <c r="BO7" s="13"/>
+      <c r="BP7" s="13"/>
+      <c r="BQ7" s="13"/>
+      <c r="BR7" s="13"/>
+      <c r="BS7" s="13"/>
+      <c r="BT7" s="13"/>
+      <c r="BU7" s="13"/>
+      <c r="BV7" s="13"/>
+      <c r="BW7" s="13"/>
+      <c r="BX7" s="13"/>
+      <c r="BY7" s="13"/>
+      <c r="BZ7" s="13"/>
+      <c r="CA7" s="13"/>
+      <c r="CB7" s="13"/>
+      <c r="CC7" s="13"/>
+      <c r="CD7" s="13"/>
+      <c r="CE7" s="13"/>
+      <c r="CF7" s="13"/>
+      <c r="CG7" s="13"/>
+      <c r="CH7" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="CI7" s="15"/>
-      <c r="CJ7" s="15" t="s">
+      <c r="CI7" s="14"/>
+      <c r="CJ7" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="CK7" s="15"/>
-      <c r="CL7" s="15"/>
-      <c r="CM7" s="15" t="s">
+      <c r="CK7" s="14"/>
+      <c r="CL7" s="14"/>
+      <c r="CM7" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="CN7" s="15"/>
+      <c r="CN7" s="14"/>
     </row>
     <row r="8" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -2463,13 +2524,13 @@
       <c r="H8" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="J8" s="13"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -2497,64 +2558,64 @@
       <c r="AL8" s="6"/>
       <c r="AM8" s="6"/>
       <c r="AN8" s="1"/>
-      <c r="AO8" s="14"/>
-      <c r="AP8" s="14"/>
-      <c r="AQ8" s="14"/>
-      <c r="AR8" s="14"/>
-      <c r="AS8" s="14"/>
-      <c r="AT8" s="14"/>
-      <c r="AU8" s="14"/>
-      <c r="AV8" s="14"/>
-      <c r="AW8" s="14"/>
-      <c r="AX8" s="14"/>
-      <c r="AY8" s="14"/>
-      <c r="AZ8" s="14"/>
-      <c r="BA8" s="14"/>
-      <c r="BB8" s="14"/>
-      <c r="BC8" s="14"/>
-      <c r="BD8" s="14"/>
-      <c r="BE8" s="15"/>
-      <c r="BF8" s="14"/>
-      <c r="BG8" s="14"/>
-      <c r="BH8" s="14"/>
-      <c r="BI8" s="14"/>
-      <c r="BJ8" s="14"/>
-      <c r="BK8" s="14"/>
-      <c r="BL8" s="14"/>
-      <c r="BM8" s="14"/>
-      <c r="BN8" s="14"/>
-      <c r="BO8" s="14"/>
-      <c r="BP8" s="14"/>
-      <c r="BQ8" s="14"/>
-      <c r="BR8" s="14"/>
-      <c r="BS8" s="14"/>
-      <c r="BT8" s="14"/>
-      <c r="BU8" s="14"/>
-      <c r="BV8" s="14"/>
-      <c r="BW8" s="14"/>
-      <c r="BX8" s="14"/>
-      <c r="BY8" s="14"/>
-      <c r="BZ8" s="14"/>
-      <c r="CA8" s="14"/>
-      <c r="CB8" s="14"/>
-      <c r="CC8" s="14"/>
-      <c r="CD8" s="14"/>
-      <c r="CE8" s="14"/>
-      <c r="CF8" s="14"/>
-      <c r="CG8" s="14"/>
-      <c r="CH8" s="15" t="s">
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
+      <c r="AQ8" s="13"/>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+      <c r="AW8" s="13"/>
+      <c r="AX8" s="13"/>
+      <c r="AY8" s="13"/>
+      <c r="AZ8" s="13"/>
+      <c r="BA8" s="13"/>
+      <c r="BB8" s="13"/>
+      <c r="BC8" s="13"/>
+      <c r="BD8" s="13"/>
+      <c r="BE8" s="14"/>
+      <c r="BF8" s="13"/>
+      <c r="BG8" s="13"/>
+      <c r="BH8" s="13"/>
+      <c r="BI8" s="13"/>
+      <c r="BJ8" s="13"/>
+      <c r="BK8" s="13"/>
+      <c r="BL8" s="13"/>
+      <c r="BM8" s="13"/>
+      <c r="BN8" s="13"/>
+      <c r="BO8" s="13"/>
+      <c r="BP8" s="13"/>
+      <c r="BQ8" s="13"/>
+      <c r="BR8" s="13"/>
+      <c r="BS8" s="13"/>
+      <c r="BT8" s="13"/>
+      <c r="BU8" s="13"/>
+      <c r="BV8" s="13"/>
+      <c r="BW8" s="13"/>
+      <c r="BX8" s="13"/>
+      <c r="BY8" s="13"/>
+      <c r="BZ8" s="13"/>
+      <c r="CA8" s="13"/>
+      <c r="CB8" s="13"/>
+      <c r="CC8" s="13"/>
+      <c r="CD8" s="13"/>
+      <c r="CE8" s="13"/>
+      <c r="CF8" s="13"/>
+      <c r="CG8" s="13"/>
+      <c r="CH8" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="CI8" s="15"/>
-      <c r="CJ8" s="15" t="s">
+      <c r="CI8" s="14"/>
+      <c r="CJ8" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="CK8" s="15"/>
-      <c r="CL8" s="15"/>
-      <c r="CM8" s="15" t="s">
+      <c r="CK8" s="14"/>
+      <c r="CL8" s="14"/>
+      <c r="CM8" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="CN8" s="15"/>
+      <c r="CN8" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
sogo and research smoke maintenance done
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADADD93-7F5D-4F3C-971D-A9C7B73106E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="597" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -12,17 +13,26 @@
     <sheet name="Users" sheetId="2" r:id="rId3"/>
     <sheet name="SanityTC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+  <calcPr calcId="191029"/>
+  <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="229">
   <si>
     <t>Environment</t>
   </si>
@@ -633,9 +643,6 @@
     <t>Reminder_EXE DP RA</t>
   </si>
   <si>
-    <t xml:space="preserve"> 05 not present on page.</t>
-  </si>
-  <si>
     <t>Sanity_TC5</t>
   </si>
   <si>
@@ -666,21 +673,12 @@
     <t>Email Address;Status;First Name</t>
   </si>
   <si>
-    <t xml:space="preserve"> Iframe Button not present on page.</t>
-  </si>
-  <si>
     <t>Sanity_TC8</t>
   </si>
   <si>
     <t>Test Invite</t>
   </si>
   <si>
-    <t>ruksar_k12</t>
-  </si>
-  <si>
-    <t>welcome29</t>
-  </si>
-  <si>
     <t>Sanity_TC9</t>
   </si>
   <si>
@@ -709,6 +707,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Login Button Static not present on page.</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>sogo_gmail110</t>
+  </si>
+  <si>
+    <t>Eighth8#</t>
   </si>
   <si>
     <t>PASS</t>
@@ -717,9 +724,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,15 +760,9 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -775,7 +776,7 @@
       <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -804,28 +805,8 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -916,7 +897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -941,14 +922,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1229,21 +1208,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1262,44 +1241,44 @@
         <v>93</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>183</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.google.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.google.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1323,7 +1302,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1331,15 +1310,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
@@ -1347,7 +1326,7 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1361,7 +1340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1354,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>184</v>
       </c>
@@ -1386,18 +1365,18 @@
         <v>186</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>183</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
@@ -1405,7 +1384,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019"/>
+    <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1413,16 +1392,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CP10"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
@@ -1439,7 +1418,7 @@
     <col min="94" max="94" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1717,18 +1696,18 @@
         <v>201</v>
       </c>
       <c r="CO1" s="7" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="CP1" s="7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:94">
+    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -1746,8 +1725,8 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="24" t="s">
-        <v>229</v>
+      <c r="I2" s="28" t="s">
+        <v>225</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
@@ -1903,7 +1882,7 @@
       <c r="CO2" s="1"/>
       <c r="CP2" s="1"/>
     </row>
-    <row r="3" spans="1:94">
+    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -1926,11 +1905,11 @@
       <c r="H3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="25" t="s">
-        <v>227</v>
+      <c r="I3" s="26" t="s">
+        <v>228</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="2"/>
@@ -2097,12 +2076,12 @@
       <c r="CO3" s="1"/>
       <c r="CP3" s="1"/>
     </row>
-    <row r="4" spans="1:94">
+    <row r="4" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -2120,11 +2099,11 @@
       <c r="H4" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I4" s="25" t="s">
-        <v>227</v>
+      <c r="I4" s="28" t="s">
+        <v>225</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2"/>
@@ -2225,12 +2204,12 @@
       <c r="CO4" s="1"/>
       <c r="CP4" s="1"/>
     </row>
-    <row r="5" spans="1:94">
+    <row r="5" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -2248,11 +2227,11 @@
       <c r="H5" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I5" s="25" t="s">
-        <v>227</v>
+      <c r="I5" s="28" t="s">
+        <v>225</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="2"/>
@@ -2353,12 +2332,12 @@
       <c r="CO5" s="1"/>
       <c r="CP5" s="1"/>
     </row>
-    <row r="6" spans="1:94">
+    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -2370,17 +2349,17 @@
         <v>184</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I6" s="25" t="s">
-        <v>227</v>
+      <c r="I6" s="28" t="s">
+        <v>225</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="11"/>
@@ -2462,7 +2441,7 @@
       </c>
       <c r="CI6" s="13"/>
       <c r="CJ6" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="CK6" s="13"/>
       <c r="CL6" s="13"/>
@@ -2471,12 +2450,12 @@
       <c r="CO6" s="1"/>
       <c r="CP6" s="1"/>
     </row>
-    <row r="7" spans="1:94">
+    <row r="7" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -2488,17 +2467,17 @@
         <v>184</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>227</v>
+        <v>208</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>225</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="11"/>
@@ -2591,12 +2570,12 @@
       <c r="CO7" s="1"/>
       <c r="CP7" s="1"/>
     </row>
-    <row r="8" spans="1:94">
+    <row r="8" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>13</v>
@@ -2608,17 +2587,17 @@
         <v>184</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>227</v>
+        <v>208</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>225</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
@@ -2700,23 +2679,23 @@
       </c>
       <c r="CI8" s="18"/>
       <c r="CJ8" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="CK8" s="18"/>
       <c r="CL8" s="18"/>
       <c r="CM8" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="CN8" s="18"/>
       <c r="CO8" s="1"/>
       <c r="CP8" s="1"/>
     </row>
-    <row r="9" spans="1:94">
+    <row r="9" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>3</v>
+        <v>213</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>13</v>
@@ -2728,7 +2707,7 @@
         <v>184</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
@@ -2835,12 +2814,12 @@
       <c r="CO9" s="1"/>
       <c r="CP9" s="1"/>
     </row>
-    <row r="10" spans="1:94">
+    <row r="10" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>3</v>
+        <v>215</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>13</v>
@@ -2852,15 +2831,15 @@
         <v>7</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="23" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -2898,10 +2877,10 @@
       <c r="AR10" s="1"/>
       <c r="AS10" s="1"/>
       <c r="AT10" s="21" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
@@ -2951,7 +2930,7 @@
       <c r="CM10" s="1"/>
       <c r="CN10" s="1"/>
       <c r="CO10" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="CP10" s="22">
         <f>DATE(2021,1,28)</f>
@@ -2960,7 +2939,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W2" r:id="rId1" display="test3t@aiktefs.com"/>
+    <hyperlink ref="W2" r:id="rId1" display="test3t@aiktefs.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
DAR case added for Engage
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="229">
   <si>
     <t>Environment</t>
   </si>
@@ -726,7 +726,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -775,8 +775,19 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -807,6 +818,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -897,7 +938,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -928,6 +969,10 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1725,7 +1770,7 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="32" t="s">
         <v>225</v>
       </c>
       <c r="J2" s="2"/>
@@ -2099,7 +2144,7 @@
       <c r="H4" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="32" t="s">
         <v>225</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -2227,7 +2272,7 @@
       <c r="H5" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="32" t="s">
         <v>225</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -2355,7 +2400,7 @@
       <c r="H6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="32" t="s">
         <v>225</v>
       </c>
       <c r="J6" s="11" t="s">
@@ -2473,7 +2518,7 @@
       <c r="H7" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="32" t="s">
         <v>225</v>
       </c>
       <c r="J7" s="11" t="s">
@@ -2593,7 +2638,7 @@
       <c r="H8" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="32" t="s">
         <v>225</v>
       </c>
       <c r="J8" s="15" t="s">

</xml_diff>

<commit_message>
Platform readings test cases are added
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24B3510-9166-4FFE-AE8B-A85275B48D0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="597" activeTab="2"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7875" tabRatio="597" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -12,8 +13,8 @@
     <sheet name="Users" sheetId="2" r:id="rId3"/>
     <sheet name="SanityTC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+  <calcPr calcId="181029"/>
+  <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="228">
   <si>
     <t>Environment</t>
   </si>
@@ -633,9 +634,6 @@
     <t>Reminder_EXE DP RA</t>
   </si>
   <si>
-    <t xml:space="preserve"> 05 not present on page.</t>
-  </si>
-  <si>
     <t>Sanity_TC5</t>
   </si>
   <si>
@@ -666,9 +664,6 @@
     <t>Email Address;Status;First Name</t>
   </si>
   <si>
-    <t xml:space="preserve"> Iframe Button not present on page.</t>
-  </si>
-  <si>
     <t>Sanity_TC8</t>
   </si>
   <si>
@@ -711,15 +706,15 @@
     <t xml:space="preserve"> Login Button Static not present on page.</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>SKIP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,6 +748,66 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -775,7 +830,7 @@
       <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -801,6 +856,161 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -916,7 +1126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -941,14 +1151,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="42" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="44" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="46" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="48" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1229,7 +1460,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1237,13 +1468,13 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1265,12 +1496,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1278,28 +1509,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.google.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.google.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1323,7 +1554,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1331,15 +1562,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
@@ -1347,7 +1578,7 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1361,7 +1592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1606,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>184</v>
       </c>
@@ -1389,15 +1620,15 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
@@ -1405,7 +1636,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019"/>
+    <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1413,16 +1644,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CP10"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
@@ -1439,7 +1670,7 @@
     <col min="94" max="94" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1717,18 +1948,18 @@
         <v>201</v>
       </c>
       <c r="CO1" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="CP1" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:94">
+    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -1746,8 +1977,8 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="24" t="s">
-        <v>229</v>
+      <c r="I2" s="51" t="s">
+        <v>227</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
@@ -1903,12 +2134,12 @@
       <c r="CO2" s="1"/>
       <c r="CP2" s="1"/>
     </row>
-    <row r="3" spans="1:94">
+    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -1926,11 +2157,11 @@
       <c r="H3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="51" t="s">
         <v>227</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="2"/>
@@ -2097,12 +2328,12 @@
       <c r="CO3" s="1"/>
       <c r="CP3" s="1"/>
     </row>
-    <row r="4" spans="1:94">
+    <row r="4" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -2120,11 +2351,11 @@
       <c r="H4" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="51" t="s">
         <v>227</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2"/>
@@ -2225,12 +2456,12 @@
       <c r="CO4" s="1"/>
       <c r="CP4" s="1"/>
     </row>
-    <row r="5" spans="1:94">
+    <row r="5" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -2248,11 +2479,11 @@
       <c r="H5" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="51" t="s">
         <v>227</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="2"/>
@@ -2353,12 +2584,12 @@
       <c r="CO5" s="1"/>
       <c r="CP5" s="1"/>
     </row>
-    <row r="6" spans="1:94">
+    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -2370,17 +2601,17 @@
         <v>184</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="51" t="s">
         <v>227</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="11"/>
@@ -2462,7 +2693,7 @@
       </c>
       <c r="CI6" s="13"/>
       <c r="CJ6" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="CK6" s="13"/>
       <c r="CL6" s="13"/>
@@ -2471,12 +2702,12 @@
       <c r="CO6" s="1"/>
       <c r="CP6" s="1"/>
     </row>
-    <row r="7" spans="1:94">
+    <row r="7" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -2488,17 +2719,17 @@
         <v>184</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="I7" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I7" s="51" t="s">
         <v>227</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="11"/>
@@ -2591,12 +2822,12 @@
       <c r="CO7" s="1"/>
       <c r="CP7" s="1"/>
     </row>
-    <row r="8" spans="1:94">
+    <row r="8" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>13</v>
@@ -2608,17 +2839,17 @@
         <v>184</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="I8" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I8" s="51" t="s">
         <v>227</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
@@ -2700,23 +2931,23 @@
       </c>
       <c r="CI8" s="18"/>
       <c r="CJ8" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="CK8" s="18"/>
       <c r="CL8" s="18"/>
       <c r="CM8" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="CN8" s="18"/>
       <c r="CO8" s="1"/>
       <c r="CP8" s="1"/>
     </row>
-    <row r="9" spans="1:94">
+    <row r="9" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>3</v>
+        <v>213</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>13</v>
@@ -2728,7 +2959,7 @@
         <v>184</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
@@ -2835,12 +3066,12 @@
       <c r="CO9" s="1"/>
       <c r="CP9" s="1"/>
     </row>
-    <row r="10" spans="1:94">
+    <row r="10" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>3</v>
+        <v>217</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>13</v>
@@ -2852,15 +3083,15 @@
         <v>7</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -2898,10 +3129,10 @@
       <c r="AR10" s="1"/>
       <c r="AS10" s="1"/>
       <c r="AT10" s="21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
@@ -2951,7 +3182,7 @@
       <c r="CM10" s="1"/>
       <c r="CN10" s="1"/>
       <c r="CO10" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="CP10" s="22">
         <f>DATE(2021,1,28)</f>
@@ -2960,7 +3191,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W2" r:id="rId1" display="test3t@aiktefs.com"/>
+    <hyperlink ref="W2" r:id="rId1" display="test3t@aiktefs.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Dp-Poll testcases, Survey logo testcases
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="229">
   <si>
     <t>Environment</t>
   </si>
@@ -717,7 +717,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -805,8 +805,19 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -822,6 +833,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
@@ -1042,7 +1083,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1084,6 +1125,10 @@
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1881,7 +1926,7 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="43" t="s">
         <v>227</v>
       </c>
       <c r="J2" s="13"/>
@@ -2061,7 +2106,7 @@
       <c r="H3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="39" t="s">
+      <c r="I3" s="43" t="s">
         <v>227</v>
       </c>
       <c r="J3" s="13" t="s">
@@ -2255,7 +2300,7 @@
       <c r="H4" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I4" s="39" t="s">
+      <c r="I4" s="43" t="s">
         <v>227</v>
       </c>
       <c r="J4" s="13" t="s">
@@ -2383,7 +2428,7 @@
       <c r="H5" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I5" s="39" t="s">
+      <c r="I5" s="43" t="s">
         <v>227</v>
       </c>
       <c r="J5" s="13" t="s">
@@ -2511,7 +2556,7 @@
       <c r="H6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I6" s="39" t="s">
+      <c r="I6" s="43" t="s">
         <v>227</v>
       </c>
       <c r="J6" s="13" t="s">
@@ -2629,7 +2674,7 @@
       <c r="H7" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I7" s="39" t="s">
+      <c r="I7" s="43" t="s">
         <v>227</v>
       </c>
       <c r="J7" s="13" t="s">
@@ -2749,7 +2794,7 @@
       <c r="H8" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="43" t="s">
         <v>227</v>
       </c>
       <c r="J8" s="17" t="s">

</xml_diff>

<commit_message>
header and footer test cases
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="229">
   <si>
     <t>Environment</t>
   </si>
@@ -717,7 +717,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -816,8 +816,19 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="43">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,6 +844,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
@@ -1083,7 +1124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1129,6 +1170,10 @@
     <xf numFmtId="0" fontId="15" fillId="40" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="15" fillId="42" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="44" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="46" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="48" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1926,7 +1971,7 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="47" t="s">
         <v>227</v>
       </c>
       <c r="J2" s="13"/>
@@ -2106,7 +2151,7 @@
       <c r="H3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="47" t="s">
         <v>227</v>
       </c>
       <c r="J3" s="13" t="s">
@@ -2300,7 +2345,7 @@
       <c r="H4" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="47" t="s">
         <v>227</v>
       </c>
       <c r="J4" s="13" t="s">
@@ -2428,7 +2473,7 @@
       <c r="H5" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="47" t="s">
         <v>227</v>
       </c>
       <c r="J5" s="13" t="s">
@@ -2556,7 +2601,7 @@
       <c r="H6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="47" t="s">
         <v>227</v>
       </c>
       <c r="J6" s="13" t="s">
@@ -2674,7 +2719,7 @@
       <c r="H7" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="47" t="s">
         <v>227</v>
       </c>
       <c r="J7" s="13" t="s">
@@ -2794,7 +2839,7 @@
       <c r="H8" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="I8" s="47" t="s">
         <v>227</v>
       </c>
       <c r="J8" s="17" t="s">

</xml_diff>

<commit_message>
Changed Lead and Owner from excel
</commit_message>
<xml_diff>
--- a/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
+++ b/Engage/Engage-Sanity/src/main/resources/excelfiles/Engage_Sanity.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6E0638-64AA-4387-8DC2-568A194FDD24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10E4F34-081C-4165-A61D-832684BAA363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="597" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,15 +15,23 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="227">
   <si>
     <t>Environment</t>
   </si>
@@ -64,15 +72,9 @@
     <t>Lead</t>
   </si>
   <si>
-    <t>Nadeem</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
-    <t>Sanket</t>
-  </si>
-  <si>
     <t>Test_Name</t>
   </si>
   <si>
@@ -709,15 +711,14 @@
     <t>SKIP</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>Gaurav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,84 +752,12 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="49">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -839,221 +768,6 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
@@ -1124,7 +838,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1137,43 +851,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="44" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="46" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="48" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1464,8 +1149,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1484,10 +1169,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1495,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1519,9 +1204,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1540,7 +1225,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -1566,10 +1251,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1591,27 +1276,27 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1619,10 +1304,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
@@ -1644,24 +1329,24 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="42.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="11" max="13" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="94" max="94" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="94" max="94" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:94" x14ac:dyDescent="0.25">
@@ -1675,491 +1360,491 @@
         <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="N1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="T1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AF1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AI1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="AK1" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AL1" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AM1" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AN1" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AO1" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AP1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AQ1" s="6" t="s">
-        <v>87</v>
-      </c>
       <c r="AR1" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AS1" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AT1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AU1" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="AV1" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="AW1" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY1" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="AX1" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="AY1" s="6" t="s">
+      <c r="AZ1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AZ1" s="6" t="s">
-        <v>109</v>
-      </c>
       <c r="BA1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="BB1" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="BC1" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="BB1" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="BC1" s="6" t="s">
+      <c r="BD1" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="BD1" s="6" t="s">
+      <c r="BE1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="BF1" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="BE1" s="6" t="s">
+      <c r="BG1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="BF1" s="6" t="s">
+      <c r="BH1" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="BG1" s="6" t="s">
+      <c r="BI1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="BH1" s="6" t="s">
+      <c r="BJ1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="BI1" s="6" t="s">
+      <c r="BK1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="BJ1" s="6" t="s">
+      <c r="BL1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="BK1" s="6" t="s">
+      <c r="BM1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="BL1" s="6" t="s">
+      <c r="BN1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="BM1" s="6" t="s">
+      <c r="BO1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="BN1" s="6" t="s">
+      <c r="BP1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="BO1" s="6" t="s">
+      <c r="BQ1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="BP1" s="6" t="s">
+      <c r="BR1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="BQ1" s="6" t="s">
+      <c r="BS1" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="BR1" s="6" t="s">
+      <c r="BT1" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="BS1" s="6" t="s">
+      <c r="BU1" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="BT1" s="6" t="s">
+      <c r="BV1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="BU1" s="6" t="s">
+      <c r="BW1" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="BV1" s="6" t="s">
+      <c r="BX1" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="BW1" s="6" t="s">
+      <c r="BY1" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="BX1" s="6" t="s">
+      <c r="BZ1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="BY1" s="6" t="s">
+      <c r="CA1" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="BZ1" s="6" t="s">
+      <c r="CB1" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="CA1" s="6" t="s">
+      <c r="CC1" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="CB1" s="6" t="s">
+      <c r="CD1" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="CC1" s="6" t="s">
+      <c r="CE1" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="CD1" s="6" t="s">
+      <c r="CF1" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="CE1" s="6" t="s">
+      <c r="CG1" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="CF1" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="CG1" s="6" t="s">
-        <v>143</v>
-      </c>
       <c r="CH1" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="CI1" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="CJ1" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="CK1" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="CL1" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="CL1" s="6" t="s">
+      <c r="CM1" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="CM1" s="6" t="s">
-        <v>194</v>
-      </c>
       <c r="CN1" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="CO1" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="CP1" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>226</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>226</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="13"/>
+      <c r="M2" s="12"/>
       <c r="N2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="AF2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AH2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AI2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AK2" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="AL2" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AN2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="AO2" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP2" s="14" t="s">
+      <c r="AP2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ2" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="AQ2" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="AR2" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="AS2" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT2" s="14"/>
-      <c r="AU2" s="14"/>
-      <c r="AV2" s="14"/>
-      <c r="AW2" s="14"/>
-      <c r="AX2" s="14"/>
-      <c r="AY2" s="14"/>
-      <c r="AZ2" s="14"/>
-      <c r="BA2" s="14"/>
-      <c r="BB2" s="14"/>
-      <c r="BC2" s="14"/>
-      <c r="BD2" s="14"/>
-      <c r="BE2" s="14"/>
-      <c r="BF2" s="14"/>
-      <c r="BG2" s="14"/>
-      <c r="BH2" s="14"/>
-      <c r="BI2" s="14"/>
-      <c r="BJ2" s="14"/>
-      <c r="BK2" s="14"/>
-      <c r="BL2" s="14"/>
-      <c r="BM2" s="14"/>
-      <c r="BN2" s="14"/>
-      <c r="BO2" s="14"/>
-      <c r="BP2" s="14"/>
-      <c r="BQ2" s="14"/>
-      <c r="BR2" s="14"/>
-      <c r="BS2" s="14"/>
-      <c r="BT2" s="14"/>
-      <c r="BU2" s="14"/>
-      <c r="BV2" s="14"/>
-      <c r="BW2" s="14"/>
-      <c r="BX2" s="14"/>
-      <c r="BY2" s="14"/>
-      <c r="BZ2" s="14"/>
-      <c r="CA2" s="14"/>
-      <c r="CB2" s="14"/>
-      <c r="CC2" s="14"/>
-      <c r="CD2" s="14"/>
-      <c r="CE2" s="14"/>
-      <c r="CF2" s="14"/>
-      <c r="CG2" s="14"/>
-      <c r="CH2" s="14"/>
-      <c r="CI2" s="14"/>
-      <c r="CJ2" s="14"/>
-      <c r="CK2" s="14"/>
-      <c r="CL2" s="14"/>
-      <c r="CM2" s="14"/>
-      <c r="CN2" s="14"/>
+      <c r="AR2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT2" s="13"/>
+      <c r="AU2" s="13"/>
+      <c r="AV2" s="13"/>
+      <c r="AW2" s="13"/>
+      <c r="AX2" s="13"/>
+      <c r="AY2" s="13"/>
+      <c r="AZ2" s="13"/>
+      <c r="BA2" s="13"/>
+      <c r="BB2" s="13"/>
+      <c r="BC2" s="13"/>
+      <c r="BD2" s="13"/>
+      <c r="BE2" s="13"/>
+      <c r="BF2" s="13"/>
+      <c r="BG2" s="13"/>
+      <c r="BH2" s="13"/>
+      <c r="BI2" s="13"/>
+      <c r="BJ2" s="13"/>
+      <c r="BK2" s="13"/>
+      <c r="BL2" s="13"/>
+      <c r="BM2" s="13"/>
+      <c r="BN2" s="13"/>
+      <c r="BO2" s="13"/>
+      <c r="BP2" s="13"/>
+      <c r="BQ2" s="13"/>
+      <c r="BR2" s="13"/>
+      <c r="BS2" s="13"/>
+      <c r="BT2" s="13"/>
+      <c r="BU2" s="13"/>
+      <c r="BV2" s="13"/>
+      <c r="BW2" s="13"/>
+      <c r="BX2" s="13"/>
+      <c r="BY2" s="13"/>
+      <c r="BZ2" s="13"/>
+      <c r="CA2" s="13"/>
+      <c r="CB2" s="13"/>
+      <c r="CC2" s="13"/>
+      <c r="CD2" s="13"/>
+      <c r="CE2" s="13"/>
+      <c r="CF2" s="13"/>
+      <c r="CG2" s="13"/>
+      <c r="CH2" s="13"/>
+      <c r="CI2" s="13"/>
+      <c r="CJ2" s="13"/>
+      <c r="CK2" s="13"/>
+      <c r="CL2" s="13"/>
+      <c r="CM2" s="13"/>
+      <c r="CN2" s="13"/>
       <c r="CO2" s="1"/>
       <c r="CP2" s="1"/>
     </row>
     <row r="3" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>226</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>226</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I3" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>226</v>
+        <v>99</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -2187,173 +1872,173 @@
       <c r="AL3" s="5"/>
       <c r="AM3" s="5"/>
       <c r="AN3" s="1"/>
-      <c r="AO3" s="14"/>
-      <c r="AP3" s="14"/>
-      <c r="AQ3" s="14"/>
-      <c r="AR3" s="14"/>
-      <c r="AS3" s="14"/>
-      <c r="AT3" s="14" t="s">
+      <c r="AO3" s="13"/>
+      <c r="AP3" s="13"/>
+      <c r="AQ3" s="13"/>
+      <c r="AR3" s="13"/>
+      <c r="AS3" s="13"/>
+      <c r="AT3" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV3" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="AU3" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="AV3" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="AW3" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="AX3" s="14" t="s">
+      <c r="AW3" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AX3" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AY3" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="BB3" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="BC3" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="BD3" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="BE3" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="BF3" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="BG3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="BH3" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="BI3" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="BJ3" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="BK3" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="BL3" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="BM3" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN3" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="BO3" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="BP3" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="BQ3" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="BR3" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="BS3" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="BT3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="BU3" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="BV3" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="BW3" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="BX3" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="BY3" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="AY3" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="AZ3" s="14" t="s">
+      <c r="BZ3" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="CA3" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="CB3" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="CC3" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="CD3" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="CE3" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="BA3" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="BB3" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="BC3" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="BD3" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="BE3" s="16" t="s">
+      <c r="CF3" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="BF3" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="BG3" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="BH3" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="BI3" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="BJ3" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="BK3" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="BL3" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="BM3" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="BN3" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="BO3" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="BP3" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="BQ3" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="BR3" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="BS3" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="BT3" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="BU3" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="BV3" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="BW3" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="BX3" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="BY3" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="BZ3" s="14" t="s">
+      <c r="CG3" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="CA3" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="CB3" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="CC3" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="CD3" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="CE3" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="CF3" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="CG3" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="CH3" s="14"/>
-      <c r="CI3" s="14"/>
-      <c r="CJ3" s="14"/>
-      <c r="CK3" s="14"/>
-      <c r="CL3" s="14"/>
-      <c r="CM3" s="14"/>
-      <c r="CN3" s="14"/>
+      <c r="CH3" s="13"/>
+      <c r="CI3" s="13"/>
+      <c r="CJ3" s="13"/>
+      <c r="CK3" s="13"/>
+      <c r="CL3" s="13"/>
+      <c r="CM3" s="13"/>
+      <c r="CN3" s="13"/>
       <c r="CO3" s="1"/>
       <c r="CP3" s="1"/>
     </row>
     <row r="4" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>226</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>226</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I4" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>226</v>
+        <v>178</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -2381,107 +2066,107 @@
       <c r="AL4" s="5"/>
       <c r="AM4" s="5"/>
       <c r="AN4" s="1"/>
-      <c r="AO4" s="14"/>
-      <c r="AP4" s="14"/>
-      <c r="AQ4" s="14"/>
-      <c r="AR4" s="14"/>
-      <c r="AS4" s="14"/>
-      <c r="AT4" s="14"/>
-      <c r="AU4" s="14"/>
-      <c r="AV4" s="14"/>
-      <c r="AW4" s="14"/>
-      <c r="AX4" s="14"/>
-      <c r="AY4" s="14"/>
-      <c r="AZ4" s="14"/>
-      <c r="BA4" s="14"/>
-      <c r="BB4" s="14"/>
-      <c r="BC4" s="14"/>
-      <c r="BD4" s="14"/>
-      <c r="BE4" s="16"/>
-      <c r="BF4" s="14"/>
-      <c r="BG4" s="14"/>
-      <c r="BH4" s="14"/>
-      <c r="BI4" s="14"/>
-      <c r="BJ4" s="14"/>
-      <c r="BK4" s="14"/>
-      <c r="BL4" s="14"/>
-      <c r="BM4" s="14"/>
-      <c r="BN4" s="14"/>
-      <c r="BO4" s="14"/>
-      <c r="BP4" s="14"/>
-      <c r="BQ4" s="14"/>
-      <c r="BR4" s="14"/>
-      <c r="BS4" s="14"/>
-      <c r="BT4" s="14"/>
-      <c r="BU4" s="14"/>
-      <c r="BV4" s="14"/>
-      <c r="BW4" s="14"/>
-      <c r="BX4" s="14"/>
-      <c r="BY4" s="14"/>
-      <c r="BZ4" s="14"/>
-      <c r="CA4" s="14"/>
-      <c r="CB4" s="14"/>
-      <c r="CC4" s="14"/>
-      <c r="CD4" s="14"/>
-      <c r="CE4" s="14"/>
-      <c r="CF4" s="14"/>
-      <c r="CG4" s="14"/>
+      <c r="AO4" s="13"/>
+      <c r="AP4" s="13"/>
+      <c r="AQ4" s="13"/>
+      <c r="AR4" s="13"/>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="13"/>
+      <c r="AW4" s="13"/>
+      <c r="AX4" s="13"/>
+      <c r="AY4" s="13"/>
+      <c r="AZ4" s="13"/>
+      <c r="BA4" s="13"/>
+      <c r="BB4" s="13"/>
+      <c r="BC4" s="13"/>
+      <c r="BD4" s="13"/>
+      <c r="BE4" s="14"/>
+      <c r="BF4" s="13"/>
+      <c r="BG4" s="13"/>
+      <c r="BH4" s="13"/>
+      <c r="BI4" s="13"/>
+      <c r="BJ4" s="13"/>
+      <c r="BK4" s="13"/>
+      <c r="BL4" s="13"/>
+      <c r="BM4" s="13"/>
+      <c r="BN4" s="13"/>
+      <c r="BO4" s="13"/>
+      <c r="BP4" s="13"/>
+      <c r="BQ4" s="13"/>
+      <c r="BR4" s="13"/>
+      <c r="BS4" s="13"/>
+      <c r="BT4" s="13"/>
+      <c r="BU4" s="13"/>
+      <c r="BV4" s="13"/>
+      <c r="BW4" s="13"/>
+      <c r="BX4" s="13"/>
+      <c r="BY4" s="13"/>
+      <c r="BZ4" s="13"/>
+      <c r="CA4" s="13"/>
+      <c r="CB4" s="13"/>
+      <c r="CC4" s="13"/>
+      <c r="CD4" s="13"/>
+      <c r="CE4" s="13"/>
+      <c r="CF4" s="13"/>
+      <c r="CG4" s="13"/>
       <c r="CH4" s="1">
         <v>282</v>
       </c>
-      <c r="CI4" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="CJ4" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="CK4" s="16" t="s">
+      <c r="CI4" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="CJ4" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="CK4" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="CL4" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="CL4" s="16" t="s">
+      <c r="CM4" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="CM4" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="CN4" s="16" t="s">
-        <v>202</v>
+      <c r="CN4" s="14" t="s">
+        <v>200</v>
       </c>
       <c r="CO4" s="1"/>
       <c r="CP4" s="1"/>
     </row>
     <row r="5" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I5" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>226</v>
+        <v>178</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -2509,107 +2194,107 @@
       <c r="AL5" s="5"/>
       <c r="AM5" s="5"/>
       <c r="AN5" s="1"/>
-      <c r="AO5" s="14"/>
-      <c r="AP5" s="14"/>
-      <c r="AQ5" s="14"/>
-      <c r="AR5" s="14"/>
-      <c r="AS5" s="14"/>
-      <c r="AT5" s="14"/>
-      <c r="AU5" s="14"/>
-      <c r="AV5" s="14"/>
-      <c r="AW5" s="14"/>
-      <c r="AX5" s="14"/>
-      <c r="AY5" s="14"/>
-      <c r="AZ5" s="14"/>
-      <c r="BA5" s="14"/>
-      <c r="BB5" s="14"/>
-      <c r="BC5" s="14"/>
-      <c r="BD5" s="14"/>
-      <c r="BE5" s="16"/>
-      <c r="BF5" s="14"/>
-      <c r="BG5" s="14"/>
-      <c r="BH5" s="14"/>
-      <c r="BI5" s="14"/>
-      <c r="BJ5" s="14"/>
-      <c r="BK5" s="14"/>
-      <c r="BL5" s="14"/>
-      <c r="BM5" s="14"/>
-      <c r="BN5" s="14"/>
-      <c r="BO5" s="14"/>
-      <c r="BP5" s="14"/>
-      <c r="BQ5" s="14"/>
-      <c r="BR5" s="14"/>
-      <c r="BS5" s="14"/>
-      <c r="BT5" s="14"/>
-      <c r="BU5" s="14"/>
-      <c r="BV5" s="14"/>
-      <c r="BW5" s="14"/>
-      <c r="BX5" s="14"/>
-      <c r="BY5" s="14"/>
-      <c r="BZ5" s="14"/>
-      <c r="CA5" s="14"/>
-      <c r="CB5" s="14"/>
-      <c r="CC5" s="14"/>
-      <c r="CD5" s="14"/>
-      <c r="CE5" s="14"/>
-      <c r="CF5" s="14"/>
-      <c r="CG5" s="14"/>
+      <c r="AO5" s="13"/>
+      <c r="AP5" s="13"/>
+      <c r="AQ5" s="13"/>
+      <c r="AR5" s="13"/>
+      <c r="AS5" s="13"/>
+      <c r="AT5" s="13"/>
+      <c r="AU5" s="13"/>
+      <c r="AV5" s="13"/>
+      <c r="AW5" s="13"/>
+      <c r="AX5" s="13"/>
+      <c r="AY5" s="13"/>
+      <c r="AZ5" s="13"/>
+      <c r="BA5" s="13"/>
+      <c r="BB5" s="13"/>
+      <c r="BC5" s="13"/>
+      <c r="BD5" s="13"/>
+      <c r="BE5" s="14"/>
+      <c r="BF5" s="13"/>
+      <c r="BG5" s="13"/>
+      <c r="BH5" s="13"/>
+      <c r="BI5" s="13"/>
+      <c r="BJ5" s="13"/>
+      <c r="BK5" s="13"/>
+      <c r="BL5" s="13"/>
+      <c r="BM5" s="13"/>
+      <c r="BN5" s="13"/>
+      <c r="BO5" s="13"/>
+      <c r="BP5" s="13"/>
+      <c r="BQ5" s="13"/>
+      <c r="BR5" s="13"/>
+      <c r="BS5" s="13"/>
+      <c r="BT5" s="13"/>
+      <c r="BU5" s="13"/>
+      <c r="BV5" s="13"/>
+      <c r="BW5" s="13"/>
+      <c r="BX5" s="13"/>
+      <c r="BY5" s="13"/>
+      <c r="BZ5" s="13"/>
+      <c r="CA5" s="13"/>
+      <c r="CB5" s="13"/>
+      <c r="CC5" s="13"/>
+      <c r="CD5" s="13"/>
+      <c r="CE5" s="13"/>
+      <c r="CF5" s="13"/>
+      <c r="CG5" s="13"/>
       <c r="CH5" s="1">
         <v>283</v>
       </c>
-      <c r="CI5" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ5" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="CK5" s="16" t="s">
+      <c r="CI5" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="CJ5" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="CK5" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="CL5" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="CL5" s="16" t="s">
+      <c r="CM5" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="CM5" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="CN5" s="16" t="s">
-        <v>199</v>
+      <c r="CN5" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="CO5" s="1"/>
       <c r="CP5" s="1"/>
     </row>
     <row r="6" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>226</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>226</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I6" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>226</v>
+        <v>178</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -2637,97 +2322,97 @@
       <c r="AL6" s="5"/>
       <c r="AM6" s="5"/>
       <c r="AN6" s="1"/>
-      <c r="AO6" s="14"/>
-      <c r="AP6" s="14"/>
-      <c r="AQ6" s="14"/>
-      <c r="AR6" s="14"/>
-      <c r="AS6" s="14"/>
-      <c r="AT6" s="14"/>
-      <c r="AU6" s="14"/>
-      <c r="AV6" s="14"/>
-      <c r="AW6" s="14"/>
-      <c r="AX6" s="14"/>
-      <c r="AY6" s="14"/>
-      <c r="AZ6" s="14"/>
-      <c r="BA6" s="14"/>
-      <c r="BB6" s="14"/>
-      <c r="BC6" s="14"/>
-      <c r="BD6" s="14"/>
-      <c r="BE6" s="16"/>
-      <c r="BF6" s="14"/>
-      <c r="BG6" s="14"/>
-      <c r="BH6" s="14"/>
-      <c r="BI6" s="14"/>
-      <c r="BJ6" s="14"/>
-      <c r="BK6" s="14"/>
-      <c r="BL6" s="14"/>
-      <c r="BM6" s="14"/>
-      <c r="BN6" s="14"/>
-      <c r="BO6" s="14"/>
-      <c r="BP6" s="14"/>
-      <c r="BQ6" s="14"/>
-      <c r="BR6" s="14"/>
-      <c r="BS6" s="14"/>
-      <c r="BT6" s="14"/>
-      <c r="BU6" s="14"/>
-      <c r="BV6" s="14"/>
-      <c r="BW6" s="14"/>
-      <c r="BX6" s="14"/>
-      <c r="BY6" s="14"/>
-      <c r="BZ6" s="14"/>
-      <c r="CA6" s="14"/>
-      <c r="CB6" s="14"/>
-      <c r="CC6" s="14"/>
-      <c r="CD6" s="14"/>
-      <c r="CE6" s="14"/>
-      <c r="CF6" s="14"/>
-      <c r="CG6" s="14"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+      <c r="AX6" s="13"/>
+      <c r="AY6" s="13"/>
+      <c r="AZ6" s="13"/>
+      <c r="BA6" s="13"/>
+      <c r="BB6" s="13"/>
+      <c r="BC6" s="13"/>
+      <c r="BD6" s="13"/>
+      <c r="BE6" s="14"/>
+      <c r="BF6" s="13"/>
+      <c r="BG6" s="13"/>
+      <c r="BH6" s="13"/>
+      <c r="BI6" s="13"/>
+      <c r="BJ6" s="13"/>
+      <c r="BK6" s="13"/>
+      <c r="BL6" s="13"/>
+      <c r="BM6" s="13"/>
+      <c r="BN6" s="13"/>
+      <c r="BO6" s="13"/>
+      <c r="BP6" s="13"/>
+      <c r="BQ6" s="13"/>
+      <c r="BR6" s="13"/>
+      <c r="BS6" s="13"/>
+      <c r="BT6" s="13"/>
+      <c r="BU6" s="13"/>
+      <c r="BV6" s="13"/>
+      <c r="BW6" s="13"/>
+      <c r="BX6" s="13"/>
+      <c r="BY6" s="13"/>
+      <c r="BZ6" s="13"/>
+      <c r="CA6" s="13"/>
+      <c r="CB6" s="13"/>
+      <c r="CC6" s="13"/>
+      <c r="CD6" s="13"/>
+      <c r="CE6" s="13"/>
+      <c r="CF6" s="13"/>
+      <c r="CG6" s="13"/>
       <c r="CH6" s="1">
         <v>283</v>
       </c>
-      <c r="CI6" s="16"/>
-      <c r="CJ6" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="CK6" s="16"/>
-      <c r="CL6" s="16"/>
-      <c r="CM6" s="16"/>
-      <c r="CN6" s="16"/>
+      <c r="CI6" s="14"/>
+      <c r="CJ6" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="CK6" s="14"/>
+      <c r="CL6" s="14"/>
+      <c r="CM6" s="14"/>
+      <c r="CN6" s="14"/>
       <c r="CO6" s="1"/>
       <c r="CP6" s="1"/>
     </row>
     <row r="7" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>226</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>226</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="I7" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>226</v>
+        <v>206</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -2755,99 +2440,99 @@
       <c r="AL7" s="5"/>
       <c r="AM7" s="5"/>
       <c r="AN7" s="1"/>
-      <c r="AO7" s="14"/>
-      <c r="AP7" s="14"/>
-      <c r="AQ7" s="14"/>
-      <c r="AR7" s="14"/>
-      <c r="AS7" s="14"/>
-      <c r="AT7" s="14"/>
-      <c r="AU7" s="14"/>
-      <c r="AV7" s="14"/>
-      <c r="AW7" s="14"/>
-      <c r="AX7" s="14"/>
-      <c r="AY7" s="14"/>
-      <c r="AZ7" s="14"/>
-      <c r="BA7" s="14"/>
-      <c r="BB7" s="14"/>
-      <c r="BC7" s="14"/>
-      <c r="BD7" s="14"/>
-      <c r="BE7" s="16"/>
-      <c r="BF7" s="14"/>
-      <c r="BG7" s="14"/>
-      <c r="BH7" s="14"/>
-      <c r="BI7" s="14"/>
-      <c r="BJ7" s="14"/>
-      <c r="BK7" s="14"/>
-      <c r="BL7" s="14"/>
-      <c r="BM7" s="14"/>
-      <c r="BN7" s="14"/>
-      <c r="BO7" s="14"/>
-      <c r="BP7" s="14"/>
-      <c r="BQ7" s="14"/>
-      <c r="BR7" s="14"/>
-      <c r="BS7" s="14"/>
-      <c r="BT7" s="14"/>
-      <c r="BU7" s="14"/>
-      <c r="BV7" s="14"/>
-      <c r="BW7" s="14"/>
-      <c r="BX7" s="14"/>
-      <c r="BY7" s="14"/>
-      <c r="BZ7" s="14"/>
-      <c r="CA7" s="14"/>
-      <c r="CB7" s="14"/>
-      <c r="CC7" s="14"/>
-      <c r="CD7" s="14"/>
-      <c r="CE7" s="14"/>
-      <c r="CF7" s="14"/>
-      <c r="CG7" s="14"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+      <c r="AX7" s="13"/>
+      <c r="AY7" s="13"/>
+      <c r="AZ7" s="13"/>
+      <c r="BA7" s="13"/>
+      <c r="BB7" s="13"/>
+      <c r="BC7" s="13"/>
+      <c r="BD7" s="13"/>
+      <c r="BE7" s="14"/>
+      <c r="BF7" s="13"/>
+      <c r="BG7" s="13"/>
+      <c r="BH7" s="13"/>
+      <c r="BI7" s="13"/>
+      <c r="BJ7" s="13"/>
+      <c r="BK7" s="13"/>
+      <c r="BL7" s="13"/>
+      <c r="BM7" s="13"/>
+      <c r="BN7" s="13"/>
+      <c r="BO7" s="13"/>
+      <c r="BP7" s="13"/>
+      <c r="BQ7" s="13"/>
+      <c r="BR7" s="13"/>
+      <c r="BS7" s="13"/>
+      <c r="BT7" s="13"/>
+      <c r="BU7" s="13"/>
+      <c r="BV7" s="13"/>
+      <c r="BW7" s="13"/>
+      <c r="BX7" s="13"/>
+      <c r="BY7" s="13"/>
+      <c r="BZ7" s="13"/>
+      <c r="CA7" s="13"/>
+      <c r="CB7" s="13"/>
+      <c r="CC7" s="13"/>
+      <c r="CD7" s="13"/>
+      <c r="CE7" s="13"/>
+      <c r="CF7" s="13"/>
+      <c r="CG7" s="13"/>
       <c r="CH7" s="1">
         <v>283</v>
       </c>
-      <c r="CI7" s="16"/>
-      <c r="CJ7" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="CK7" s="16"/>
-      <c r="CL7" s="16"/>
-      <c r="CM7" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="CN7" s="16"/>
+      <c r="CI7" s="14"/>
+      <c r="CJ7" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="CK7" s="14"/>
+      <c r="CL7" s="14"/>
+      <c r="CM7" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="CN7" s="14"/>
       <c r="CO7" s="1"/>
       <c r="CP7" s="1"/>
     </row>
     <row r="8" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>15</v>
+        <v>181</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="I8" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>226</v>
+        <v>206</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>224</v>
       </c>
       <c r="K8" s="8"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
@@ -2875,89 +2560,89 @@
       <c r="AL8" s="9"/>
       <c r="AM8" s="9"/>
       <c r="AN8" s="8"/>
-      <c r="AO8" s="18"/>
-      <c r="AP8" s="18"/>
-      <c r="AQ8" s="18"/>
-      <c r="AR8" s="18"/>
-      <c r="AS8" s="18"/>
-      <c r="AT8" s="18"/>
-      <c r="AU8" s="18"/>
-      <c r="AV8" s="18"/>
-      <c r="AW8" s="18"/>
-      <c r="AX8" s="18"/>
-      <c r="AY8" s="18"/>
-      <c r="AZ8" s="18"/>
-      <c r="BA8" s="18"/>
-      <c r="BB8" s="18"/>
-      <c r="BC8" s="18"/>
-      <c r="BD8" s="18"/>
-      <c r="BE8" s="19"/>
-      <c r="BF8" s="18"/>
-      <c r="BG8" s="18"/>
-      <c r="BH8" s="18"/>
-      <c r="BI8" s="18"/>
-      <c r="BJ8" s="18"/>
-      <c r="BK8" s="18"/>
-      <c r="BL8" s="18"/>
-      <c r="BM8" s="18"/>
-      <c r="BN8" s="18"/>
-      <c r="BO8" s="18"/>
-      <c r="BP8" s="18"/>
-      <c r="BQ8" s="18"/>
-      <c r="BR8" s="18"/>
-      <c r="BS8" s="18"/>
-      <c r="BT8" s="18"/>
-      <c r="BU8" s="18"/>
-      <c r="BV8" s="18"/>
-      <c r="BW8" s="18"/>
-      <c r="BX8" s="18"/>
-      <c r="BY8" s="18"/>
-      <c r="BZ8" s="18"/>
-      <c r="CA8" s="18"/>
-      <c r="CB8" s="18"/>
-      <c r="CC8" s="18"/>
-      <c r="CD8" s="18"/>
-      <c r="CE8" s="18"/>
-      <c r="CF8" s="18"/>
-      <c r="CG8" s="18"/>
+      <c r="AO8" s="16"/>
+      <c r="AP8" s="16"/>
+      <c r="AQ8" s="16"/>
+      <c r="AR8" s="16"/>
+      <c r="AS8" s="16"/>
+      <c r="AT8" s="16"/>
+      <c r="AU8" s="16"/>
+      <c r="AV8" s="16"/>
+      <c r="AW8" s="16"/>
+      <c r="AX8" s="16"/>
+      <c r="AY8" s="16"/>
+      <c r="AZ8" s="16"/>
+      <c r="BA8" s="16"/>
+      <c r="BB8" s="16"/>
+      <c r="BC8" s="16"/>
+      <c r="BD8" s="16"/>
+      <c r="BE8" s="17"/>
+      <c r="BF8" s="16"/>
+      <c r="BG8" s="16"/>
+      <c r="BH8" s="16"/>
+      <c r="BI8" s="16"/>
+      <c r="BJ8" s="16"/>
+      <c r="BK8" s="16"/>
+      <c r="BL8" s="16"/>
+      <c r="BM8" s="16"/>
+      <c r="BN8" s="16"/>
+      <c r="BO8" s="16"/>
+      <c r="BP8" s="16"/>
+      <c r="BQ8" s="16"/>
+      <c r="BR8" s="16"/>
+      <c r="BS8" s="16"/>
+      <c r="BT8" s="16"/>
+      <c r="BU8" s="16"/>
+      <c r="BV8" s="16"/>
+      <c r="BW8" s="16"/>
+      <c r="BX8" s="16"/>
+      <c r="BY8" s="16"/>
+      <c r="BZ8" s="16"/>
+      <c r="CA8" s="16"/>
+      <c r="CB8" s="16"/>
+      <c r="CC8" s="16"/>
+      <c r="CD8" s="16"/>
+      <c r="CE8" s="16"/>
+      <c r="CF8" s="16"/>
+      <c r="CG8" s="16"/>
       <c r="CH8" s="1">
         <v>283</v>
       </c>
-      <c r="CI8" s="19"/>
-      <c r="CJ8" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="CK8" s="19"/>
-      <c r="CL8" s="19"/>
-      <c r="CM8" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="CN8" s="19"/>
+      <c r="CI8" s="17"/>
+      <c r="CJ8" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="CK8" s="17"/>
+      <c r="CL8" s="17"/>
+      <c r="CM8" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="CN8" s="17"/>
       <c r="CO8" s="1"/>
       <c r="CP8" s="1"/>
     </row>
     <row r="9" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>214</v>
+        <v>181</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>212</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3039,53 +2724,53 @@
       <c r="CH9" s="1">
         <v>283</v>
       </c>
-      <c r="CI9" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ9" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="CK9" s="16" t="s">
+      <c r="CI9" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="CJ9" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="CK9" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="CL9" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="CL9" s="16" t="s">
+      <c r="CM9" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="CM9" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="CN9" s="16" t="s">
-        <v>199</v>
+      <c r="CN9" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="CO9" s="1"/>
       <c r="CP9" s="1"/>
     </row>
     <row r="10" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>217</v>
+      <c r="A10" s="13" t="s">
+        <v>215</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>218</v>
+      <c r="F10" s="13" t="s">
+        <v>216</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="20" t="s">
-        <v>225</v>
+      <c r="I10" s="18" t="s">
+        <v>223</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -3123,10 +2808,10 @@
       <c r="AR10" s="1"/>
       <c r="AS10" s="1"/>
       <c r="AT10" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
@@ -3166,7 +2851,7 @@
       <c r="CE10" s="1"/>
       <c r="CF10" s="1"/>
       <c r="CG10" s="1"/>
-      <c r="CH10" s="14">
+      <c r="CH10" s="13">
         <v>91</v>
       </c>
       <c r="CI10" s="1"/>
@@ -3176,7 +2861,7 @@
       <c r="CM10" s="1"/>
       <c r="CN10" s="1"/>
       <c r="CO10" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="CP10" s="11">
         <f>DATE(2021,1,28)</f>

</xml_diff>